<commit_message>
"reajuste do periodo e das funções, sem transformações especiais"
</commit_message>
<xml_diff>
--- a/Data/final_data.xlsx
+++ b/Data/final_data.xlsx
@@ -474,7 +474,7 @@
         <v>1980.042</v>
       </c>
       <c r="E2" t="n">
-        <v>0.52</v>
+        <v>0.37</v>
       </c>
       <c r="F2" t="n">
         <v>338.55</v>
@@ -494,7 +494,7 @@
         <v>1980.125</v>
       </c>
       <c r="E3" t="n">
-        <v>0.43</v>
+        <v>0.46</v>
       </c>
       <c r="F3" t="n">
         <v>339.26</v>
@@ -514,7 +514,7 @@
         <v>1980.208</v>
       </c>
       <c r="E4" t="n">
-        <v>0.47</v>
+        <v>0.35</v>
       </c>
       <c r="F4" t="n">
         <v>339.59</v>
@@ -554,7 +554,7 @@
         <v>1980.375</v>
       </c>
       <c r="E6" t="n">
-        <v>0.28</v>
+        <v>0.39</v>
       </c>
       <c r="F6" t="n">
         <v>340.44</v>
@@ -574,7 +574,7 @@
         <v>1980.458</v>
       </c>
       <c r="E7" t="n">
-        <v>0.33</v>
+        <v>0.27</v>
       </c>
       <c r="F7" t="n">
         <v>339.99</v>
@@ -594,7 +594,7 @@
         <v>1980.542</v>
       </c>
       <c r="E8" t="n">
-        <v>0.32</v>
+        <v>0.31</v>
       </c>
       <c r="F8" t="n">
         <v>338.44</v>
@@ -614,7 +614,7 @@
         <v>1980.625</v>
       </c>
       <c r="E9" t="n">
-        <v>0.34</v>
+        <v>0.28</v>
       </c>
       <c r="F9" t="n">
         <v>337.21</v>
@@ -634,7 +634,7 @@
         <v>1980.708</v>
       </c>
       <c r="E10" t="n">
-        <v>0.22</v>
+        <v>0.25</v>
       </c>
       <c r="F10" t="n">
         <v>337.05</v>
@@ -654,7 +654,7 @@
         <v>1980.792</v>
       </c>
       <c r="E11" t="n">
-        <v>0.25</v>
+        <v>0.19</v>
       </c>
       <c r="F11" t="n">
         <v>337.83</v>
@@ -674,7 +674,7 @@
         <v>1980.875</v>
       </c>
       <c r="E12" t="n">
-        <v>0.29</v>
+        <v>0.26</v>
       </c>
       <c r="F12" t="n">
         <v>338.93</v>
@@ -694,7 +694,7 @@
         <v>1980.958</v>
       </c>
       <c r="E13" t="n">
-        <v>0.46</v>
+        <v>0.23</v>
       </c>
       <c r="F13" t="n">
         <v>339.64</v>
@@ -714,7 +714,7 @@
         <v>1981.042</v>
       </c>
       <c r="E14" t="n">
-        <v>0.09</v>
+        <v>0.52</v>
       </c>
       <c r="F14" t="n">
         <v>340.18</v>
@@ -734,7 +734,7 @@
         <v>1981.125</v>
       </c>
       <c r="E15" t="n">
-        <v>0.21</v>
+        <v>0.43</v>
       </c>
       <c r="F15" t="n">
         <v>340.75</v>
@@ -754,7 +754,7 @@
         <v>1981.208</v>
       </c>
       <c r="E16" t="n">
-        <v>0.05</v>
+        <v>0.47</v>
       </c>
       <c r="F16" t="n">
         <v>341.38</v>
@@ -774,7 +774,7 @@
         <v>1981.292</v>
       </c>
       <c r="E17" t="n">
-        <v>0.15</v>
+        <v>0.34</v>
       </c>
       <c r="F17" t="n">
         <v>341.68</v>
@@ -794,7 +794,7 @@
         <v>1981.375</v>
       </c>
       <c r="E18" t="n">
-        <v>0.17</v>
+        <v>0.28</v>
       </c>
       <c r="F18" t="n">
         <v>341.43</v>
@@ -814,7 +814,7 @@
         <v>1981.458</v>
       </c>
       <c r="E19" t="n">
-        <v>0.1</v>
+        <v>0.33</v>
       </c>
       <c r="F19" t="n">
         <v>340.63</v>
@@ -834,7 +834,7 @@
         <v>1981.542</v>
       </c>
       <c r="E20" t="n">
-        <v>0.18</v>
+        <v>0.32</v>
       </c>
       <c r="F20" t="n">
         <v>339.22</v>
@@ -854,7 +854,7 @@
         <v>1981.625</v>
       </c>
       <c r="E21" t="n">
-        <v>0.11</v>
+        <v>0.34</v>
       </c>
       <c r="F21" t="n">
         <v>338.08</v>
@@ -874,7 +874,7 @@
         <v>1981.708</v>
       </c>
       <c r="E22" t="n">
-        <v>0.2</v>
+        <v>0.22</v>
       </c>
       <c r="F22" t="n">
         <v>337.98</v>
@@ -894,7 +894,7 @@
         <v>1981.792</v>
       </c>
       <c r="E23" t="n">
-        <v>0.16</v>
+        <v>0.25</v>
       </c>
       <c r="F23" t="n">
         <v>339.07</v>
@@ -914,7 +914,7 @@
         <v>1981.875</v>
       </c>
       <c r="E24" t="n">
-        <v>0.16</v>
+        <v>0.29</v>
       </c>
       <c r="F24" t="n">
         <v>340.18</v>
@@ -934,7 +934,7 @@
         <v>1981.958</v>
       </c>
       <c r="E25" t="n">
-        <v>0.44</v>
+        <v>0.46</v>
       </c>
       <c r="F25" t="n">
         <v>340.75</v>
@@ -954,7 +954,7 @@
         <v>1982.042</v>
       </c>
       <c r="E26" t="n">
-        <v>0.49</v>
+        <v>0.09</v>
       </c>
       <c r="F26" t="n">
         <v>341.37</v>
@@ -974,7 +974,7 @@
         <v>1982.125</v>
       </c>
       <c r="E27" t="n">
-        <v>0.45</v>
+        <v>0.21</v>
       </c>
       <c r="F27" t="n">
         <v>341.95</v>
@@ -994,7 +994,7 @@
         <v>1982.208</v>
       </c>
       <c r="E28" t="n">
-        <v>0.42</v>
+        <v>0.05</v>
       </c>
       <c r="F28" t="n">
         <v>342.23</v>
@@ -1014,7 +1014,7 @@
         <v>1982.292</v>
       </c>
       <c r="E29" t="n">
-        <v>0.28</v>
+        <v>0.15</v>
       </c>
       <c r="F29" t="n">
         <v>342.52</v>
@@ -1034,7 +1034,7 @@
         <v>1982.375</v>
       </c>
       <c r="E30" t="n">
-        <v>0.37</v>
+        <v>0.17</v>
       </c>
       <c r="F30" t="n">
         <v>342.36</v>
@@ -1054,7 +1054,7 @@
         <v>1982.458</v>
       </c>
       <c r="E31" t="n">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
       <c r="F31" t="n">
         <v>341.49</v>
@@ -1074,7 +1074,7 @@
         <v>1982.542</v>
       </c>
       <c r="E32" t="n">
-        <v>0.23</v>
+        <v>0.18</v>
       </c>
       <c r="F32" t="n">
         <v>339.75</v>
@@ -1094,7 +1094,7 @@
         <v>1982.625</v>
       </c>
       <c r="E33" t="n">
-        <v>0.36</v>
+        <v>0.11</v>
       </c>
       <c r="F33" t="n">
         <v>338.11</v>
@@ -1114,7 +1114,7 @@
         <v>1982.708</v>
       </c>
       <c r="E34" t="n">
-        <v>0.42</v>
+        <v>0.2</v>
       </c>
       <c r="F34" t="n">
         <v>338.16</v>
@@ -1134,7 +1134,7 @@
         <v>1982.792</v>
       </c>
       <c r="E35" t="n">
-        <v>0.22</v>
+        <v>0.16</v>
       </c>
       <c r="F35" t="n">
         <v>339.62</v>
@@ -1154,7 +1154,7 @@
         <v>1982.875</v>
       </c>
       <c r="E36" t="n">
-        <v>0.35</v>
+        <v>0.16</v>
       </c>
       <c r="F36" t="n">
         <v>340.95</v>
@@ -1174,7 +1174,7 @@
         <v>1982.958</v>
       </c>
       <c r="E37" t="n">
-        <v>0.23</v>
+        <v>0.44</v>
       </c>
       <c r="F37" t="n">
         <v>341.77</v>
@@ -1194,7 +1194,7 @@
         <v>1983.042</v>
       </c>
       <c r="E38" t="n">
-        <v>0.3</v>
+        <v>0.49</v>
       </c>
       <c r="F38" t="n">
         <v>342.37</v>
@@ -1214,7 +1214,7 @@
         <v>1983.125</v>
       </c>
       <c r="E39" t="n">
-        <v>0.19</v>
+        <v>0.45</v>
       </c>
       <c r="F39" t="n">
         <v>342.74</v>
@@ -1234,7 +1234,7 @@
         <v>1983.208</v>
       </c>
       <c r="E40" t="n">
-        <v>0.3</v>
+        <v>0.42</v>
       </c>
       <c r="F40" t="n">
         <v>343.04</v>
@@ -1254,7 +1254,7 @@
         <v>1983.292</v>
       </c>
       <c r="E41" t="n">
-        <v>0.12</v>
+        <v>0.28</v>
       </c>
       <c r="F41" t="n">
         <v>343.51</v>
@@ -1274,7 +1274,7 @@
         <v>1983.375</v>
       </c>
       <c r="E42" t="n">
-        <v>0.36</v>
+        <v>0.37</v>
       </c>
       <c r="F42" t="n">
         <v>343.84</v>
@@ -1294,7 +1294,7 @@
         <v>1983.458</v>
       </c>
       <c r="E43" t="n">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="F43" t="n">
         <v>343.5</v>
@@ -1314,7 +1314,7 @@
         <v>1983.542</v>
       </c>
       <c r="E44" t="n">
-        <v>0.17</v>
+        <v>0.23</v>
       </c>
       <c r="F44" t="n">
         <v>342.14</v>
@@ -1334,7 +1334,7 @@
         <v>1983.625</v>
       </c>
       <c r="E45" t="n">
-        <v>0.21</v>
+        <v>0.36</v>
       </c>
       <c r="F45" t="n">
         <v>340.62</v>
@@ -1354,7 +1354,7 @@
         <v>1983.708</v>
       </c>
       <c r="E46" t="n">
-        <v>0.24</v>
+        <v>0.42</v>
       </c>
       <c r="F46" t="n">
         <v>340.53</v>
@@ -1374,7 +1374,7 @@
         <v>1983.792</v>
       </c>
       <c r="E47" t="n">
-        <v>0.16</v>
+        <v>0.22</v>
       </c>
       <c r="F47" t="n">
         <v>341.75</v>
@@ -1394,7 +1394,7 @@
         <v>1983.875</v>
       </c>
       <c r="E48" t="n">
-        <v>0.08</v>
+        <v>0.35</v>
       </c>
       <c r="F48" t="n">
         <v>342.83</v>
@@ -1414,7 +1414,7 @@
         <v>1983.958</v>
       </c>
       <c r="E49" t="n">
-        <v>0.01</v>
+        <v>0.23</v>
       </c>
       <c r="F49" t="n">
         <v>343.49</v>
@@ -1434,7 +1434,7 @@
         <v>1984.042</v>
       </c>
       <c r="E50" t="n">
-        <v>0.28</v>
+        <v>0.3</v>
       </c>
       <c r="F50" t="n">
         <v>344.32</v>
@@ -1454,7 +1454,7 @@
         <v>1984.125</v>
       </c>
       <c r="E51" t="n">
-        <v>0.04</v>
+        <v>0.19</v>
       </c>
       <c r="F51" t="n">
         <v>344.82</v>
@@ -1474,7 +1474,7 @@
         <v>1984.208</v>
       </c>
       <c r="E52" t="n">
-        <v>0.21</v>
+        <v>0.3</v>
       </c>
       <c r="F52" t="n">
         <v>344.96</v>
@@ -1494,7 +1494,7 @@
         <v>1984.292</v>
       </c>
       <c r="E53" t="n">
-        <v>0.14</v>
+        <v>0.12</v>
       </c>
       <c r="F53" t="n">
         <v>345.19</v>
@@ -1514,7 +1514,7 @@
         <v>1984.375</v>
       </c>
       <c r="E54" t="n">
-        <v>0.19</v>
+        <v>0.36</v>
       </c>
       <c r="F54" t="n">
         <v>345.33</v>
@@ -1534,7 +1534,7 @@
         <v>1984.458</v>
       </c>
       <c r="E55" t="n">
-        <v>0.19</v>
+        <v>0.1</v>
       </c>
       <c r="F55" t="n">
         <v>344.57</v>
@@ -1554,7 +1554,7 @@
         <v>1984.542</v>
       </c>
       <c r="E56" t="n">
-        <v>0.04</v>
+        <v>0.17</v>
       </c>
       <c r="F56" t="n">
         <v>343.2</v>
@@ -1574,7 +1574,7 @@
         <v>1984.625</v>
       </c>
       <c r="E57" t="n">
-        <v>0.17</v>
+        <v>0.21</v>
       </c>
       <c r="F57" t="n">
         <v>342.21</v>
@@ -1594,7 +1594,7 @@
         <v>1984.708</v>
       </c>
       <c r="E58" t="n">
-        <v>0.17</v>
+        <v>0.24</v>
       </c>
       <c r="F58" t="n">
         <v>342.13</v>
@@ -1614,7 +1614,7 @@
         <v>1984.792</v>
       </c>
       <c r="E59" t="n">
-        <v>0.13</v>
+        <v>0.16</v>
       </c>
       <c r="F59" t="n">
         <v>342.99</v>
@@ -1634,7 +1634,7 @@
         <v>1984.875</v>
       </c>
       <c r="E60" t="n">
-        <v>0.11</v>
+        <v>0.08</v>
       </c>
       <c r="F60" t="n">
         <v>344.16</v>
@@ -1654,7 +1654,7 @@
         <v>1984.958</v>
       </c>
       <c r="E61" t="n">
-        <v>0.19</v>
+        <v>0.01</v>
       </c>
       <c r="F61" t="n">
         <v>345</v>
@@ -1694,7 +1694,7 @@
         <v>1985.125</v>
       </c>
       <c r="E63" t="n">
-        <v>0.39</v>
+        <v>0.04</v>
       </c>
       <c r="F63" t="n">
         <v>345.8</v>
@@ -1714,7 +1714,7 @@
         <v>1985.208</v>
       </c>
       <c r="E64" t="n">
-        <v>0.3</v>
+        <v>0.21</v>
       </c>
       <c r="F64" t="n">
         <v>346.64</v>
@@ -1734,7 +1734,7 @@
         <v>1985.292</v>
       </c>
       <c r="E65" t="n">
-        <v>0.25</v>
+        <v>0.14</v>
       </c>
       <c r="F65" t="n">
         <v>346.94</v>
@@ -1754,7 +1754,7 @@
         <v>1985.375</v>
       </c>
       <c r="E66" t="n">
-        <v>0.27</v>
+        <v>0.19</v>
       </c>
       <c r="F66" t="n">
         <v>346.78</v>
@@ -1774,7 +1774,7 @@
         <v>1985.458</v>
       </c>
       <c r="E67" t="n">
-        <v>0.17</v>
+        <v>0.19</v>
       </c>
       <c r="F67" t="n">
         <v>346.26</v>
@@ -1794,7 +1794,7 @@
         <v>1985.542</v>
       </c>
       <c r="E68" t="n">
-        <v>0.17</v>
+        <v>0.04</v>
       </c>
       <c r="F68" t="n">
         <v>344.92</v>
@@ -1814,7 +1814,7 @@
         <v>1985.625</v>
       </c>
       <c r="E69" t="n">
-        <v>0.19</v>
+        <v>0.17</v>
       </c>
       <c r="F69" t="n">
         <v>343.41</v>
@@ -1834,7 +1834,7 @@
         <v>1985.708</v>
       </c>
       <c r="E70" t="n">
-        <v>0.12</v>
+        <v>0.17</v>
       </c>
       <c r="F70" t="n">
         <v>343.37</v>
@@ -1854,7 +1854,7 @@
         <v>1985.792</v>
       </c>
       <c r="E71" t="n">
-        <v>0.17</v>
+        <v>0.13</v>
       </c>
       <c r="F71" t="n">
         <v>344.64</v>
@@ -1874,7 +1874,7 @@
         <v>1985.875</v>
       </c>
       <c r="E72" t="n">
-        <v>0.13</v>
+        <v>0.11</v>
       </c>
       <c r="F72" t="n">
         <v>345.79</v>
@@ -1894,7 +1894,7 @@
         <v>1985.958</v>
       </c>
       <c r="E73" t="n">
-        <v>0.21</v>
+        <v>0.19</v>
       </c>
       <c r="F73" t="n">
         <v>346.55</v>
@@ -1914,7 +1914,7 @@
         <v>1986.042</v>
       </c>
       <c r="E74" t="n">
-        <v>0.34</v>
+        <v>0.28</v>
       </c>
       <c r="F74" t="n">
         <v>347.11</v>
@@ -1934,7 +1934,7 @@
         <v>1986.125</v>
       </c>
       <c r="E75" t="n">
-        <v>0.38</v>
+        <v>0.39</v>
       </c>
       <c r="F75" t="n">
         <v>347.34</v>
@@ -1954,7 +1954,7 @@
         <v>1986.208</v>
       </c>
       <c r="E76" t="n">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="F76" t="n">
         <v>347.71</v>
@@ -1974,7 +1974,7 @@
         <v>1986.292</v>
       </c>
       <c r="E77" t="n">
-        <v>0.26</v>
+        <v>0.25</v>
       </c>
       <c r="F77" t="n">
         <v>348.22</v>
@@ -1994,7 +1994,7 @@
         <v>1986.375</v>
       </c>
       <c r="E78" t="n">
-        <v>0.31</v>
+        <v>0.27</v>
       </c>
       <c r="F78" t="n">
         <v>348.32</v>
@@ -2014,7 +2014,7 @@
         <v>1986.458</v>
       </c>
       <c r="E79" t="n">
-        <v>0.36</v>
+        <v>0.17</v>
       </c>
       <c r="F79" t="n">
         <v>347.76</v>
@@ -2034,7 +2034,7 @@
         <v>1986.542</v>
       </c>
       <c r="E80" t="n">
-        <v>0.48</v>
+        <v>0.17</v>
       </c>
       <c r="F80" t="n">
         <v>346.29</v>
@@ -2054,7 +2054,7 @@
         <v>1986.625</v>
       </c>
       <c r="E81" t="n">
-        <v>0.31</v>
+        <v>0.19</v>
       </c>
       <c r="F81" t="n">
         <v>344.92</v>
@@ -2074,7 +2074,7 @@
         <v>1986.708</v>
       </c>
       <c r="E82" t="n">
-        <v>0.4</v>
+        <v>0.12</v>
       </c>
       <c r="F82" t="n">
         <v>344.86</v>
@@ -2094,7 +2094,7 @@
         <v>1986.792</v>
       </c>
       <c r="E83" t="n">
-        <v>0.33</v>
+        <v>0.17</v>
       </c>
       <c r="F83" t="n">
         <v>346.03</v>
@@ -2114,7 +2114,7 @@
         <v>1986.875</v>
       </c>
       <c r="E84" t="n">
-        <v>0.26</v>
+        <v>0.13</v>
       </c>
       <c r="F84" t="n">
         <v>347.3</v>
@@ -2134,7 +2134,7 @@
         <v>1986.958</v>
       </c>
       <c r="E85" t="n">
-        <v>0.45</v>
+        <v>0.21</v>
       </c>
       <c r="F85" t="n">
         <v>347.76</v>
@@ -2154,7 +2154,7 @@
         <v>1987.042</v>
       </c>
       <c r="E86" t="n">
-        <v>0.54</v>
+        <v>0.34</v>
       </c>
       <c r="F86" t="n">
         <v>348.02</v>
@@ -2174,7 +2174,7 @@
         <v>1987.125</v>
       </c>
       <c r="E87" t="n">
-        <v>0.46</v>
+        <v>0.38</v>
       </c>
       <c r="F87" t="n">
         <v>348.57</v>
@@ -2194,7 +2194,7 @@
         <v>1987.208</v>
       </c>
       <c r="E88" t="n">
-        <v>0.52</v>
+        <v>0.2</v>
       </c>
       <c r="F88" t="n">
         <v>349.29</v>
@@ -2214,7 +2214,7 @@
         <v>1987.292</v>
       </c>
       <c r="E89" t="n">
-        <v>0.45</v>
+        <v>0.26</v>
       </c>
       <c r="F89" t="n">
         <v>349.98</v>
@@ -2234,7 +2234,7 @@
         <v>1987.375</v>
       </c>
       <c r="E90" t="n">
-        <v>0.46</v>
+        <v>0.31</v>
       </c>
       <c r="F90" t="n">
         <v>350.26</v>
@@ -2254,7 +2254,7 @@
         <v>1987.458</v>
       </c>
       <c r="E91" t="n">
-        <v>0.43</v>
+        <v>0.36</v>
       </c>
       <c r="F91" t="n">
         <v>349.48</v>
@@ -2274,7 +2274,7 @@
         <v>1987.542</v>
       </c>
       <c r="E92" t="n">
-        <v>0.36</v>
+        <v>0.48</v>
       </c>
       <c r="F92" t="n">
         <v>347.86</v>
@@ -2294,7 +2294,7 @@
         <v>1987.625</v>
       </c>
       <c r="E93" t="n">
-        <v>0.4</v>
+        <v>0.31</v>
       </c>
       <c r="F93" t="n">
         <v>346.61</v>
@@ -2314,7 +2314,7 @@
         <v>1987.708</v>
       </c>
       <c r="E94" t="n">
-        <v>0.38</v>
+        <v>0.4</v>
       </c>
       <c r="F94" t="n">
         <v>346.7</v>
@@ -2334,7 +2334,7 @@
         <v>1987.792</v>
       </c>
       <c r="E95" t="n">
-        <v>0.36</v>
+        <v>0.33</v>
       </c>
       <c r="F95" t="n">
         <v>347.97</v>
@@ -2354,7 +2354,7 @@
         <v>1987.875</v>
       </c>
       <c r="E96" t="n">
-        <v>0.14</v>
+        <v>0.26</v>
       </c>
       <c r="F96" t="n">
         <v>349.25</v>
@@ -2374,7 +2374,7 @@
         <v>1987.958</v>
       </c>
       <c r="E97" t="n">
-        <v>0.28</v>
+        <v>0.45</v>
       </c>
       <c r="F97" t="n">
         <v>350.21</v>
@@ -2394,7 +2394,7 @@
         <v>1988.042</v>
       </c>
       <c r="E98" t="n">
-        <v>0.1</v>
+        <v>0.54</v>
       </c>
       <c r="F98" t="n">
         <v>350.91</v>
@@ -2414,7 +2414,7 @@
         <v>1988.125</v>
       </c>
       <c r="E99" t="n">
-        <v>0.32</v>
+        <v>0.46</v>
       </c>
       <c r="F99" t="n">
         <v>351.47</v>
@@ -2434,7 +2434,7 @@
         <v>1988.208</v>
       </c>
       <c r="E100" t="n">
-        <v>0.32</v>
+        <v>0.52</v>
       </c>
       <c r="F100" t="n">
         <v>351.85</v>
@@ -2454,7 +2454,7 @@
         <v>1988.292</v>
       </c>
       <c r="E101" t="n">
-        <v>0.31</v>
+        <v>0.45</v>
       </c>
       <c r="F101" t="n">
         <v>352.3</v>
@@ -2474,7 +2474,7 @@
         <v>1988.375</v>
       </c>
       <c r="E102" t="n">
-        <v>0.2</v>
+        <v>0.46</v>
       </c>
       <c r="F102" t="n">
         <v>352.46</v>
@@ -2494,7 +2494,7 @@
         <v>1988.458</v>
       </c>
       <c r="E103" t="n">
-        <v>0.22</v>
+        <v>0.43</v>
       </c>
       <c r="F103" t="n">
         <v>351.76</v>
@@ -2514,7 +2514,7 @@
         <v>1988.542</v>
       </c>
       <c r="E104" t="n">
-        <v>0.3</v>
+        <v>0.36</v>
       </c>
       <c r="F104" t="n">
         <v>350.28</v>
@@ -2534,7 +2534,7 @@
         <v>1988.625</v>
       </c>
       <c r="E105" t="n">
-        <v>0.33</v>
+        <v>0.4</v>
       </c>
       <c r="F105" t="n">
         <v>349.1</v>
@@ -2554,7 +2554,7 @@
         <v>1988.708</v>
       </c>
       <c r="E106" t="n">
-        <v>0.39</v>
+        <v>0.38</v>
       </c>
       <c r="F106" t="n">
         <v>349.27</v>
@@ -2574,7 +2574,7 @@
         <v>1988.792</v>
       </c>
       <c r="E107" t="n">
-        <v>0.31</v>
+        <v>0.36</v>
       </c>
       <c r="F107" t="n">
         <v>350.44</v>
@@ -2594,7 +2594,7 @@
         <v>1988.875</v>
       </c>
       <c r="E108" t="n">
-        <v>0.17</v>
+        <v>0.14</v>
       </c>
       <c r="F108" t="n">
         <v>351.61</v>
@@ -2614,7 +2614,7 @@
         <v>1988.958</v>
       </c>
       <c r="E109" t="n">
-        <v>0.41</v>
+        <v>0.28</v>
       </c>
       <c r="F109" t="n">
         <v>352.46</v>
@@ -2634,7 +2634,7 @@
         <v>1989.042</v>
       </c>
       <c r="E110" t="n">
-        <v>0.38</v>
+        <v>0.1</v>
       </c>
       <c r="F110" t="n">
         <v>352.99</v>
@@ -2654,7 +2654,7 @@
         <v>1989.125</v>
       </c>
       <c r="E111" t="n">
-        <v>0.38</v>
+        <v>0.32</v>
       </c>
       <c r="F111" t="n">
         <v>353.46</v>
@@ -2674,7 +2674,7 @@
         <v>1989.208</v>
       </c>
       <c r="E112" t="n">
-        <v>0.75</v>
+        <v>0.32</v>
       </c>
       <c r="F112" t="n">
         <v>354</v>
@@ -2694,7 +2694,7 @@
         <v>1989.292</v>
       </c>
       <c r="E113" t="n">
-        <v>0.61</v>
+        <v>0.31</v>
       </c>
       <c r="F113" t="n">
         <v>354.38</v>
@@ -2714,7 +2714,7 @@
         <v>1989.375</v>
       </c>
       <c r="E114" t="n">
-        <v>0.51</v>
+        <v>0.2</v>
       </c>
       <c r="F114" t="n">
         <v>354.19</v>
@@ -2734,7 +2734,7 @@
         <v>1989.458</v>
       </c>
       <c r="E115" t="n">
-        <v>0.39</v>
+        <v>0.22</v>
       </c>
       <c r="F115" t="n">
         <v>353.26</v>
@@ -2754,7 +2754,7 @@
         <v>1989.542</v>
       </c>
       <c r="E116" t="n">
-        <v>0.41</v>
+        <v>0.3</v>
       </c>
       <c r="F116" t="n">
         <v>351.56</v>
@@ -2774,7 +2774,7 @@
         <v>1989.625</v>
       </c>
       <c r="E117" t="n">
-        <v>0.35</v>
+        <v>0.33</v>
       </c>
       <c r="F117" t="n">
         <v>350.21</v>
@@ -2794,7 +2794,7 @@
         <v>1989.708</v>
       </c>
       <c r="E118" t="n">
-        <v>0.32</v>
+        <v>0.39</v>
       </c>
       <c r="F118" t="n">
         <v>350.56</v>
@@ -2814,7 +2814,7 @@
         <v>1989.792</v>
       </c>
       <c r="E119" t="n">
-        <v>0.42</v>
+        <v>0.31</v>
       </c>
       <c r="F119" t="n">
         <v>351.85</v>
@@ -2834,7 +2834,7 @@
         <v>1989.875</v>
       </c>
       <c r="E120" t="n">
-        <v>0.41</v>
+        <v>0.17</v>
       </c>
       <c r="F120" t="n">
         <v>353.04</v>
@@ -2874,7 +2874,7 @@
         <v>1990.042</v>
       </c>
       <c r="E122" t="n">
-        <v>0.4</v>
+        <v>0.38</v>
       </c>
       <c r="F122" t="n">
         <v>354.46</v>
@@ -2894,7 +2894,7 @@
         <v>1990.125</v>
       </c>
       <c r="E123" t="n">
-        <v>0.5</v>
+        <v>0.38</v>
       </c>
       <c r="F123" t="n">
         <v>354.87</v>
@@ -2914,7 +2914,7 @@
         <v>1990.208</v>
       </c>
       <c r="E124" t="n">
-        <v>0.37</v>
+        <v>0.75</v>
       </c>
       <c r="F124" t="n">
         <v>355.2</v>
@@ -2934,7 +2934,7 @@
         <v>1990.292</v>
       </c>
       <c r="E125" t="n">
-        <v>0.52</v>
+        <v>0.61</v>
       </c>
       <c r="F125" t="n">
         <v>355.5</v>
@@ -2954,7 +2954,7 @@
         <v>1990.375</v>
       </c>
       <c r="E126" t="n">
-        <v>0.42</v>
+        <v>0.51</v>
       </c>
       <c r="F126" t="n">
         <v>355.4</v>
@@ -2974,7 +2974,7 @@
         <v>1990.458</v>
       </c>
       <c r="E127" t="n">
-        <v>0.54</v>
+        <v>0.39</v>
       </c>
       <c r="F127" t="n">
         <v>354.33</v>
@@ -2994,7 +2994,7 @@
         <v>1990.542</v>
       </c>
       <c r="E128" t="n">
-        <v>0.48</v>
+        <v>0.41</v>
       </c>
       <c r="F128" t="n">
         <v>352.71</v>
@@ -3014,7 +3014,7 @@
         <v>1990.625</v>
       </c>
       <c r="E129" t="n">
-        <v>0.41</v>
+        <v>0.35</v>
       </c>
       <c r="F129" t="n">
         <v>351.59</v>
@@ -3034,7 +3034,7 @@
         <v>1990.708</v>
       </c>
       <c r="E130" t="n">
-        <v>0.42</v>
+        <v>0.32</v>
       </c>
       <c r="F130" t="n">
         <v>351.8</v>
@@ -3054,7 +3054,7 @@
         <v>1990.792</v>
       </c>
       <c r="E131" t="n">
-        <v>0.32</v>
+        <v>0.42</v>
       </c>
       <c r="F131" t="n">
         <v>353.19</v>
@@ -3074,7 +3074,7 @@
         <v>1990.875</v>
       </c>
       <c r="E132" t="n">
-        <v>0.3</v>
+        <v>0.41</v>
       </c>
       <c r="F132" t="n">
         <v>354.43</v>
@@ -3094,7 +3094,7 @@
         <v>1990.958</v>
       </c>
       <c r="E133" t="n">
-        <v>0.29</v>
+        <v>0.41</v>
       </c>
       <c r="F133" t="n">
         <v>355.18</v>
@@ -3114,7 +3114,7 @@
         <v>1991.042</v>
       </c>
       <c r="E134" t="n">
-        <v>0.43</v>
+        <v>0.4</v>
       </c>
       <c r="F134" t="n">
         <v>355.76</v>
@@ -3134,7 +3134,7 @@
         <v>1991.125</v>
       </c>
       <c r="E135" t="n">
-        <v>0.43</v>
+        <v>0.5</v>
       </c>
       <c r="F135" t="n">
         <v>356.19</v>
@@ -3154,7 +3154,7 @@
         <v>1991.208</v>
       </c>
       <c r="E136" t="n">
-        <v>0.47</v>
+        <v>0.37</v>
       </c>
       <c r="F136" t="n">
         <v>356.68</v>
@@ -3174,7 +3174,7 @@
         <v>1991.292</v>
       </c>
       <c r="E137" t="n">
-        <v>0.29</v>
+        <v>0.52</v>
       </c>
       <c r="F137" t="n">
         <v>357.19</v>
@@ -3194,7 +3194,7 @@
         <v>1991.375</v>
       </c>
       <c r="E138" t="n">
-        <v>0.34</v>
+        <v>0.42</v>
       </c>
       <c r="F138" t="n">
         <v>357.11</v>
@@ -3214,7 +3214,7 @@
         <v>1991.458</v>
       </c>
       <c r="E139" t="n">
-        <v>0.29</v>
+        <v>0.54</v>
       </c>
       <c r="F139" t="n">
         <v>356.17</v>
@@ -3234,7 +3234,7 @@
         <v>1991.542</v>
       </c>
       <c r="E140" t="n">
-        <v>0.14</v>
+        <v>0.48</v>
       </c>
       <c r="F140" t="n">
         <v>354.53</v>
@@ -3254,7 +3254,7 @@
         <v>1991.625</v>
       </c>
       <c r="E141" t="n">
-        <v>0.1</v>
+        <v>0.41</v>
       </c>
       <c r="F141" t="n">
         <v>353.05</v>
@@ -3274,7 +3274,7 @@
         <v>1991.708</v>
       </c>
       <c r="E142" t="n">
-        <v>0.03</v>
+        <v>0.42</v>
       </c>
       <c r="F142" t="n">
         <v>352.93</v>
@@ -3294,7 +3294,7 @@
         <v>1991.792</v>
       </c>
       <c r="E143" t="n">
-        <v>0.06</v>
+        <v>0.32</v>
       </c>
       <c r="F143" t="n">
         <v>354</v>
@@ -3314,7 +3314,7 @@
         <v>1991.875</v>
       </c>
       <c r="E144" t="n">
-        <v>0.04</v>
+        <v>0.3</v>
       </c>
       <c r="F144" t="n">
         <v>355.16</v>
@@ -3334,7 +3334,7 @@
         <v>1991.958</v>
       </c>
       <c r="E145" t="n">
-        <v>0.2</v>
+        <v>0.29</v>
       </c>
       <c r="F145" t="n">
         <v>355.95</v>
@@ -3354,7 +3354,7 @@
         <v>1992.042</v>
       </c>
       <c r="E146" t="n">
-        <v>0.33</v>
+        <v>0.43</v>
       </c>
       <c r="F146" t="n">
         <v>356.52</v>
@@ -3374,7 +3374,7 @@
         <v>1992.125</v>
       </c>
       <c r="E147" t="n">
-        <v>0.39</v>
+        <v>0.43</v>
       </c>
       <c r="F147" t="n">
         <v>356.89</v>
@@ -3394,7 +3394,7 @@
         <v>1992.208</v>
       </c>
       <c r="E148" t="n">
-        <v>0.36</v>
+        <v>0.47</v>
       </c>
       <c r="F148" t="n">
         <v>357.26</v>
@@ -3414,7 +3414,7 @@
         <v>1992.292</v>
       </c>
       <c r="E149" t="n">
-        <v>0.32</v>
+        <v>0.29</v>
       </c>
       <c r="F149" t="n">
         <v>357.75</v>
@@ -3434,7 +3434,7 @@
         <v>1992.375</v>
       </c>
       <c r="E150" t="n">
-        <v>0.3</v>
+        <v>0.34</v>
       </c>
       <c r="F150" t="n">
         <v>357.82</v>
@@ -3454,7 +3454,7 @@
         <v>1992.458</v>
       </c>
       <c r="E151" t="n">
-        <v>0.31</v>
+        <v>0.29</v>
       </c>
       <c r="F151" t="n">
         <v>356.87</v>
@@ -3474,7 +3474,7 @@
         <v>1992.542</v>
       </c>
       <c r="E152" t="n">
-        <v>0.26</v>
+        <v>0.14</v>
       </c>
       <c r="F152" t="n">
         <v>355.19</v>
@@ -3494,7 +3494,7 @@
         <v>1992.625</v>
       </c>
       <c r="E153" t="n">
-        <v>0.18</v>
+        <v>0.1</v>
       </c>
       <c r="F153" t="n">
         <v>353.68</v>
@@ -3514,7 +3514,7 @@
         <v>1992.708</v>
       </c>
       <c r="E154" t="n">
-        <v>0.19</v>
+        <v>0.03</v>
       </c>
       <c r="F154" t="n">
         <v>353.58</v>
@@ -3534,7 +3534,7 @@
         <v>1992.792</v>
       </c>
       <c r="E155" t="n">
-        <v>0.25</v>
+        <v>0.06</v>
       </c>
       <c r="F155" t="n">
         <v>354.8</v>
@@ -3554,7 +3554,7 @@
         <v>1992.875</v>
       </c>
       <c r="E156" t="n">
-        <v>0.08</v>
+        <v>0.04</v>
       </c>
       <c r="F156" t="n">
         <v>355.98</v>
@@ -3594,7 +3594,7 @@
         <v>1993.042</v>
       </c>
       <c r="E158" t="n">
-        <v>0.22</v>
+        <v>0.33</v>
       </c>
       <c r="F158" t="n">
         <v>357.21</v>
@@ -3614,7 +3614,7 @@
         <v>1993.125</v>
       </c>
       <c r="E159" t="n">
-        <v>0.06</v>
+        <v>0.39</v>
       </c>
       <c r="F159" t="n">
         <v>357.55</v>
@@ -3634,7 +3634,7 @@
         <v>1993.208</v>
       </c>
       <c r="E160" t="n">
-        <v>0.3</v>
+        <v>0.36</v>
       </c>
       <c r="F160" t="n">
         <v>357.96</v>
@@ -3654,7 +3654,7 @@
         <v>1993.292</v>
       </c>
       <c r="E161" t="n">
-        <v>0.39</v>
+        <v>0.32</v>
       </c>
       <c r="F161" t="n">
         <v>358.43</v>
@@ -3674,7 +3674,7 @@
         <v>1993.375</v>
       </c>
       <c r="E162" t="n">
-        <v>0.33</v>
+        <v>0.3</v>
       </c>
       <c r="F162" t="n">
         <v>358.38</v>
@@ -3694,7 +3694,7 @@
         <v>1993.458</v>
       </c>
       <c r="E163" t="n">
-        <v>0.43</v>
+        <v>0.31</v>
       </c>
       <c r="F163" t="n">
         <v>357.34</v>
@@ -3714,7 +3714,7 @@
         <v>1993.542</v>
       </c>
       <c r="E164" t="n">
-        <v>0.32</v>
+        <v>0.26</v>
       </c>
       <c r="F164" t="n">
         <v>355.72</v>
@@ -3734,7 +3734,7 @@
         <v>1993.625</v>
       </c>
       <c r="E165" t="n">
-        <v>0.24</v>
+        <v>0.18</v>
       </c>
       <c r="F165" t="n">
         <v>354.44</v>
@@ -3754,7 +3754,7 @@
         <v>1993.708</v>
       </c>
       <c r="E166" t="n">
-        <v>0.35</v>
+        <v>0.19</v>
       </c>
       <c r="F166" t="n">
         <v>354.47</v>
@@ -3774,7 +3774,7 @@
         <v>1993.792</v>
       </c>
       <c r="E167" t="n">
-        <v>0.44</v>
+        <v>0.25</v>
       </c>
       <c r="F167" t="n">
         <v>355.7</v>
@@ -3794,7 +3794,7 @@
         <v>1993.875</v>
       </c>
       <c r="E168" t="n">
-        <v>0.43</v>
+        <v>0.08</v>
       </c>
       <c r="F168" t="n">
         <v>356.95</v>
@@ -3814,7 +3814,7 @@
         <v>1993.958</v>
       </c>
       <c r="E169" t="n">
-        <v>0.38</v>
+        <v>0.2</v>
       </c>
       <c r="F169" t="n">
         <v>357.85</v>
@@ -3834,7 +3834,7 @@
         <v>1994.042</v>
       </c>
       <c r="E170" t="n">
-        <v>0.54</v>
+        <v>0.22</v>
       </c>
       <c r="F170" t="n">
         <v>358.47</v>
@@ -3854,7 +3854,7 @@
         <v>1994.125</v>
       </c>
       <c r="E171" t="n">
-        <v>0.76</v>
+        <v>0.06</v>
       </c>
       <c r="F171" t="n">
         <v>359.01</v>
@@ -3874,7 +3874,7 @@
         <v>1994.208</v>
       </c>
       <c r="E172" t="n">
-        <v>0.51</v>
+        <v>0.3</v>
       </c>
       <c r="F172" t="n">
         <v>359.36</v>
@@ -3894,7 +3894,7 @@
         <v>1994.292</v>
       </c>
       <c r="E173" t="n">
-        <v>0.5</v>
+        <v>0.39</v>
       </c>
       <c r="F173" t="n">
         <v>359.71</v>
@@ -3934,7 +3934,7 @@
         <v>1994.458</v>
       </c>
       <c r="E175" t="n">
-        <v>0.46</v>
+        <v>0.43</v>
       </c>
       <c r="F175" t="n">
         <v>358.81</v>
@@ -3954,7 +3954,7 @@
         <v>1994.542</v>
       </c>
       <c r="E176" t="n">
-        <v>0.49</v>
+        <v>0.32</v>
       </c>
       <c r="F176" t="n">
         <v>357.27</v>
@@ -3974,7 +3974,7 @@
         <v>1994.625</v>
       </c>
       <c r="E177" t="n">
-        <v>0.53</v>
+        <v>0.24</v>
       </c>
       <c r="F177" t="n">
         <v>356.05</v>
@@ -3994,7 +3994,7 @@
         <v>1994.708</v>
       </c>
       <c r="E178" t="n">
-        <v>0.41</v>
+        <v>0.35</v>
       </c>
       <c r="F178" t="n">
         <v>356.02</v>
@@ -4014,7 +4014,7 @@
         <v>1994.792</v>
       </c>
       <c r="E179" t="n">
-        <v>0.43</v>
+        <v>0.44</v>
       </c>
       <c r="F179" t="n">
         <v>357.26</v>
@@ -4034,7 +4034,7 @@
         <v>1994.875</v>
       </c>
       <c r="E180" t="n">
-        <v>0.46</v>
+        <v>0.43</v>
       </c>
       <c r="F180" t="n">
         <v>358.69</v>
@@ -4054,7 +4054,7 @@
         <v>1994.958</v>
       </c>
       <c r="E181" t="n">
-        <v>0.3</v>
+        <v>0.38</v>
       </c>
       <c r="F181" t="n">
         <v>359.55</v>
@@ -4074,7 +4074,7 @@
         <v>1995.042</v>
       </c>
       <c r="E182" t="n">
-        <v>0.27</v>
+        <v>0.54</v>
       </c>
       <c r="F182" t="n">
         <v>360.13</v>
@@ -4094,7 +4094,7 @@
         <v>1995.125</v>
       </c>
       <c r="E183" t="n">
-        <v>0.49</v>
+        <v>0.76</v>
       </c>
       <c r="F183" t="n">
         <v>360.61</v>
@@ -4114,7 +4114,7 @@
         <v>1995.208</v>
       </c>
       <c r="E184" t="n">
-        <v>0.38</v>
+        <v>0.51</v>
       </c>
       <c r="F184" t="n">
         <v>361.08</v>
@@ -4134,7 +4134,7 @@
         <v>1995.292</v>
       </c>
       <c r="E185" t="n">
-        <v>0.34</v>
+        <v>0.5</v>
       </c>
       <c r="F185" t="n">
         <v>361.55</v>
@@ -4174,7 +4174,7 @@
         <v>1995.458</v>
       </c>
       <c r="E187" t="n">
-        <v>0.29</v>
+        <v>0.46</v>
       </c>
       <c r="F187" t="n">
         <v>360.61</v>
@@ -4194,7 +4194,7 @@
         <v>1995.542</v>
       </c>
       <c r="E188" t="n">
-        <v>0.37</v>
+        <v>0.49</v>
       </c>
       <c r="F188" t="n">
         <v>358.99</v>
@@ -4214,7 +4214,7 @@
         <v>1995.625</v>
       </c>
       <c r="E189" t="n">
-        <v>0.45</v>
+        <v>0.53</v>
       </c>
       <c r="F189" t="n">
         <v>357.73</v>
@@ -4234,7 +4234,7 @@
         <v>1995.708</v>
       </c>
       <c r="E190" t="n">
-        <v>0.28</v>
+        <v>0.41</v>
       </c>
       <c r="F190" t="n">
         <v>358.05</v>
@@ -4254,7 +4254,7 @@
         <v>1995.792</v>
       </c>
       <c r="E191" t="n">
-        <v>0.2</v>
+        <v>0.43</v>
       </c>
       <c r="F191" t="n">
         <v>359.42</v>
@@ -4274,7 +4274,7 @@
         <v>1995.875</v>
       </c>
       <c r="E192" t="n">
-        <v>0.39</v>
+        <v>0.46</v>
       </c>
       <c r="F192" t="n">
         <v>360.77</v>
@@ -4294,7 +4294,7 @@
         <v>1995.958</v>
       </c>
       <c r="E193" t="n">
-        <v>0.36</v>
+        <v>0.3</v>
       </c>
       <c r="F193" t="n">
         <v>361.65</v>
@@ -4314,7 +4314,7 @@
         <v>1996.042</v>
       </c>
       <c r="E194" t="n">
-        <v>0.26</v>
+        <v>0.27</v>
       </c>
       <c r="F194" t="n">
         <v>362.14</v>
@@ -4334,7 +4334,7 @@
         <v>1996.125</v>
       </c>
       <c r="E195" t="n">
-        <v>0.37</v>
+        <v>0.49</v>
       </c>
       <c r="F195" t="n">
         <v>362.5</v>
@@ -4354,7 +4354,7 @@
         <v>1996.208</v>
       </c>
       <c r="E196" t="n">
-        <v>0.51</v>
+        <v>0.38</v>
       </c>
       <c r="F196" t="n">
         <v>362.82</v>
@@ -4374,7 +4374,7 @@
         <v>1996.292</v>
       </c>
       <c r="E197" t="n">
-        <v>0.39</v>
+        <v>0.34</v>
       </c>
       <c r="F197" t="n">
         <v>363.14</v>
@@ -4394,7 +4394,7 @@
         <v>1996.375</v>
       </c>
       <c r="E198" t="n">
-        <v>0.39</v>
+        <v>0.33</v>
       </c>
       <c r="F198" t="n">
         <v>363.29</v>
@@ -4414,7 +4414,7 @@
         <v>1996.458</v>
       </c>
       <c r="E199" t="n">
-        <v>0.5600000000000001</v>
+        <v>0.29</v>
       </c>
       <c r="F199" t="n">
         <v>362.88</v>
@@ -4434,7 +4434,7 @@
         <v>1996.542</v>
       </c>
       <c r="E200" t="n">
-        <v>0.42</v>
+        <v>0.37</v>
       </c>
       <c r="F200" t="n">
         <v>361.57</v>
@@ -4454,7 +4454,7 @@
         <v>1996.625</v>
       </c>
       <c r="E201" t="n">
-        <v>0.46</v>
+        <v>0.45</v>
       </c>
       <c r="F201" t="n">
         <v>360.07</v>
@@ -4474,7 +4474,7 @@
         <v>1996.708</v>
       </c>
       <c r="E202" t="n">
-        <v>0.61</v>
+        <v>0.28</v>
       </c>
       <c r="F202" t="n">
         <v>359.7</v>
@@ -4494,7 +4494,7 @@
         <v>1996.792</v>
       </c>
       <c r="E203" t="n">
-        <v>0.64</v>
+        <v>0.2</v>
       </c>
       <c r="F203" t="n">
         <v>360.67</v>
@@ -4514,7 +4514,7 @@
         <v>1996.875</v>
       </c>
       <c r="E204" t="n">
-        <v>0.62</v>
+        <v>0.39</v>
       </c>
       <c r="F204" t="n">
         <v>361.78</v>
@@ -4534,7 +4534,7 @@
         <v>1996.958</v>
       </c>
       <c r="E205" t="n">
-        <v>0.58</v>
+        <v>0.36</v>
       </c>
       <c r="F205" t="n">
         <v>362.63</v>
@@ -4554,7 +4554,7 @@
         <v>1997.042</v>
       </c>
       <c r="E206" t="n">
-        <v>0.59</v>
+        <v>0.26</v>
       </c>
       <c r="F206" t="n">
         <v>363.28</v>
@@ -4574,7 +4574,7 @@
         <v>1997.125</v>
       </c>
       <c r="E207" t="n">
-        <v>0.8100000000000001</v>
+        <v>0.37</v>
       </c>
       <c r="F207" t="n">
         <v>363.65</v>
@@ -4594,7 +4594,7 @@
         <v>1997.208</v>
       </c>
       <c r="E208" t="n">
-        <v>0.64</v>
+        <v>0.51</v>
       </c>
       <c r="F208" t="n">
         <v>364.03</v>
@@ -4614,7 +4614,7 @@
         <v>1997.292</v>
       </c>
       <c r="E209" t="n">
-        <v>0.72</v>
+        <v>0.39</v>
       </c>
       <c r="F209" t="n">
         <v>364.51</v>
@@ -4634,7 +4634,7 @@
         <v>1997.375</v>
       </c>
       <c r="E210" t="n">
-        <v>0.7</v>
+        <v>0.39</v>
       </c>
       <c r="F210" t="n">
         <v>364.51</v>
@@ -4654,7 +4654,7 @@
         <v>1997.458</v>
       </c>
       <c r="E211" t="n">
-        <v>0.73</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="F211" t="n">
         <v>363.6</v>
@@ -4674,7 +4674,7 @@
         <v>1997.542</v>
       </c>
       <c r="E212" t="n">
-        <v>0.7</v>
+        <v>0.42</v>
       </c>
       <c r="F212" t="n">
         <v>361.93</v>
@@ -4694,7 +4694,7 @@
         <v>1997.625</v>
       </c>
       <c r="E213" t="n">
-        <v>0.71</v>
+        <v>0.46</v>
       </c>
       <c r="F213" t="n">
         <v>360.41</v>
@@ -4714,7 +4714,7 @@
         <v>1997.708</v>
       </c>
       <c r="E214" t="n">
-        <v>0.5</v>
+        <v>0.61</v>
       </c>
       <c r="F214" t="n">
         <v>360.41</v>
@@ -4734,7 +4734,7 @@
         <v>1997.792</v>
       </c>
       <c r="E215" t="n">
-        <v>0.44</v>
+        <v>0.64</v>
       </c>
       <c r="F215" t="n">
         <v>361.94</v>
@@ -4754,7 +4754,7 @@
         <v>1997.875</v>
       </c>
       <c r="E216" t="n">
-        <v>0.44</v>
+        <v>0.62</v>
       </c>
       <c r="F216" t="n">
         <v>363.61</v>
@@ -4794,7 +4794,7 @@
         <v>1998.042</v>
       </c>
       <c r="E218" t="n">
-        <v>0.47</v>
+        <v>0.59</v>
       </c>
       <c r="F218" t="n">
         <v>365.19</v>
@@ -4814,7 +4814,7 @@
         <v>1998.125</v>
       </c>
       <c r="E219" t="n">
-        <v>0.64</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="F219" t="n">
         <v>365.46</v>
@@ -4834,7 +4834,7 @@
         <v>1998.208</v>
       </c>
       <c r="E220" t="n">
-        <v>0.37</v>
+        <v>0.64</v>
       </c>
       <c r="F220" t="n">
         <v>365.93</v>
@@ -4854,7 +4854,7 @@
         <v>1998.292</v>
       </c>
       <c r="E221" t="n">
-        <v>0.37</v>
+        <v>0.72</v>
       </c>
       <c r="F221" t="n">
         <v>366.58</v>
@@ -4874,7 +4874,7 @@
         <v>1998.375</v>
       </c>
       <c r="E222" t="n">
-        <v>0.32</v>
+        <v>0.7</v>
       </c>
       <c r="F222" t="n">
         <v>366.86</v>
@@ -4894,7 +4894,7 @@
         <v>1998.458</v>
       </c>
       <c r="E223" t="n">
-        <v>0.41</v>
+        <v>0.73</v>
       </c>
       <c r="F223" t="n">
         <v>366.27</v>
@@ -4914,7 +4914,7 @@
         <v>1998.542</v>
       </c>
       <c r="E224" t="n">
-        <v>0.38</v>
+        <v>0.7</v>
       </c>
       <c r="F224" t="n">
         <v>364.84</v>
@@ -4934,7 +4934,7 @@
         <v>1998.625</v>
       </c>
       <c r="E225" t="n">
-        <v>0.38</v>
+        <v>0.71</v>
       </c>
       <c r="F225" t="n">
         <v>363.79</v>
@@ -4954,7 +4954,7 @@
         <v>1998.708</v>
       </c>
       <c r="E226" t="n">
-        <v>0.42</v>
+        <v>0.5</v>
       </c>
       <c r="F226" t="n">
         <v>364.04</v>
@@ -4974,7 +4974,7 @@
         <v>1998.792</v>
       </c>
       <c r="E227" t="n">
-        <v>0.34</v>
+        <v>0.44</v>
       </c>
       <c r="F227" t="n">
         <v>365.34</v>
@@ -4994,7 +4994,7 @@
         <v>1998.875</v>
       </c>
       <c r="E228" t="n">
-        <v>0.36</v>
+        <v>0.44</v>
       </c>
       <c r="F228" t="n">
         <v>366.6</v>
@@ -5014,7 +5014,7 @@
         <v>1998.958</v>
       </c>
       <c r="E229" t="n">
-        <v>0.46</v>
+        <v>0.58</v>
       </c>
       <c r="F229" t="n">
         <v>367.47</v>
@@ -5034,7 +5034,7 @@
         <v>1999.042</v>
       </c>
       <c r="E230" t="n">
-        <v>0.31</v>
+        <v>0.47</v>
       </c>
       <c r="F230" t="n">
         <v>368.12</v>
@@ -5054,7 +5054,7 @@
         <v>1999.125</v>
       </c>
       <c r="E231" t="n">
-        <v>0.55</v>
+        <v>0.64</v>
       </c>
       <c r="F231" t="n">
         <v>368.52</v>
@@ -5074,7 +5074,7 @@
         <v>1999.208</v>
       </c>
       <c r="E232" t="n">
-        <v>0.53</v>
+        <v>0.37</v>
       </c>
       <c r="F232" t="n">
         <v>368.91</v>
@@ -5094,7 +5094,7 @@
         <v>1999.292</v>
       </c>
       <c r="E233" t="n">
-        <v>0.59</v>
+        <v>0.37</v>
       </c>
       <c r="F233" t="n">
         <v>369.3</v>
@@ -5114,7 +5114,7 @@
         <v>1999.375</v>
       </c>
       <c r="E234" t="n">
-        <v>0.36</v>
+        <v>0.32</v>
       </c>
       <c r="F234" t="n">
         <v>369.21</v>
@@ -5134,7 +5134,7 @@
         <v>1999.458</v>
       </c>
       <c r="E235" t="n">
-        <v>0.38</v>
+        <v>0.41</v>
       </c>
       <c r="F235" t="n">
         <v>368.36</v>
@@ -5154,7 +5154,7 @@
         <v>1999.542</v>
       </c>
       <c r="E236" t="n">
-        <v>0.4</v>
+        <v>0.38</v>
       </c>
       <c r="F236" t="n">
         <v>366.69</v>
@@ -5174,7 +5174,7 @@
         <v>1999.625</v>
       </c>
       <c r="E237" t="n">
-        <v>0.44</v>
+        <v>0.38</v>
       </c>
       <c r="F237" t="n">
         <v>365.32</v>
@@ -5194,7 +5194,7 @@
         <v>1999.708</v>
       </c>
       <c r="E238" t="n">
-        <v>0.44</v>
+        <v>0.42</v>
       </c>
       <c r="F238" t="n">
         <v>365.44</v>
@@ -5214,7 +5214,7 @@
         <v>1999.792</v>
       </c>
       <c r="E239" t="n">
-        <v>0.31</v>
+        <v>0.34</v>
       </c>
       <c r="F239" t="n">
         <v>366.75</v>
@@ -5234,7 +5234,7 @@
         <v>1999.875</v>
       </c>
       <c r="E240" t="n">
-        <v>0.3</v>
+        <v>0.36</v>
       </c>
       <c r="F240" t="n">
         <v>368.05</v>
@@ -5254,7 +5254,7 @@
         <v>1999.958</v>
       </c>
       <c r="E241" t="n">
-        <v>0.3</v>
+        <v>0.46</v>
       </c>
       <c r="F241" t="n">
         <v>368.88</v>
@@ -5274,7 +5274,7 @@
         <v>2000.042</v>
       </c>
       <c r="E242" t="n">
-        <v>0.45</v>
+        <v>0.31</v>
       </c>
       <c r="F242" t="n">
         <v>369.39</v>
@@ -5294,7 +5294,7 @@
         <v>2000.125</v>
       </c>
       <c r="E243" t="n">
-        <v>0.43</v>
+        <v>0.55</v>
       </c>
       <c r="F243" t="n">
         <v>369.65</v>
@@ -5314,7 +5314,7 @@
         <v>2000.208</v>
       </c>
       <c r="E244" t="n">
-        <v>0.55</v>
+        <v>0.53</v>
       </c>
       <c r="F244" t="n">
         <v>369.97</v>
@@ -5334,7 +5334,7 @@
         <v>2000.292</v>
       </c>
       <c r="E245" t="n">
-        <v>0.53</v>
+        <v>0.59</v>
       </c>
       <c r="F245" t="n">
         <v>370.35</v>
@@ -5354,7 +5354,7 @@
         <v>2000.375</v>
       </c>
       <c r="E246" t="n">
-        <v>0.57</v>
+        <v>0.36</v>
       </c>
       <c r="F246" t="n">
         <v>370.24</v>
@@ -5374,7 +5374,7 @@
         <v>2000.458</v>
       </c>
       <c r="E247" t="n">
-        <v>0.53</v>
+        <v>0.38</v>
       </c>
       <c r="F247" t="n">
         <v>369.31</v>
@@ -5394,7 +5394,7 @@
         <v>2000.542</v>
       </c>
       <c r="E248" t="n">
-        <v>0.62</v>
+        <v>0.4</v>
       </c>
       <c r="F248" t="n">
         <v>367.91</v>
@@ -5414,7 +5414,7 @@
         <v>2000.625</v>
       </c>
       <c r="E249" t="n">
-        <v>0.54</v>
+        <v>0.44</v>
       </c>
       <c r="F249" t="n">
         <v>366.76</v>
@@ -5434,7 +5434,7 @@
         <v>2000.708</v>
       </c>
       <c r="E250" t="n">
-        <v>0.55</v>
+        <v>0.44</v>
       </c>
       <c r="F250" t="n">
         <v>366.71</v>
@@ -5454,7 +5454,7 @@
         <v>2000.792</v>
       </c>
       <c r="E251" t="n">
-        <v>0.49</v>
+        <v>0.31</v>
       </c>
       <c r="F251" t="n">
         <v>367.91</v>
@@ -5474,7 +5474,7 @@
         <v>2000.875</v>
       </c>
       <c r="E252" t="n">
-        <v>0.68</v>
+        <v>0.3</v>
       </c>
       <c r="F252" t="n">
         <v>369.28</v>
@@ -5494,7 +5494,7 @@
         <v>2000.958</v>
       </c>
       <c r="E253" t="n">
-        <v>0.62</v>
+        <v>0.3</v>
       </c>
       <c r="F253" t="n">
         <v>370.1</v>
@@ -5514,7 +5514,7 @@
         <v>2001.042</v>
       </c>
       <c r="E254" t="n">
-        <v>0.68</v>
+        <v>0.45</v>
       </c>
       <c r="F254" t="n">
         <v>370.69</v>
@@ -5534,7 +5534,7 @@
         <v>2001.125</v>
       </c>
       <c r="E255" t="n">
-        <v>0.68</v>
+        <v>0.43</v>
       </c>
       <c r="F255" t="n">
         <v>371.18</v>
@@ -5554,7 +5554,7 @@
         <v>2001.208</v>
       </c>
       <c r="E256" t="n">
-        <v>0.83</v>
+        <v>0.55</v>
       </c>
       <c r="F256" t="n">
         <v>371.59</v>
@@ -5574,7 +5574,7 @@
         <v>2001.292</v>
       </c>
       <c r="E257" t="n">
-        <v>0.5600000000000001</v>
+        <v>0.53</v>
       </c>
       <c r="F257" t="n">
         <v>371.9</v>
@@ -5594,7 +5594,7 @@
         <v>2001.375</v>
       </c>
       <c r="E258" t="n">
-        <v>0.65</v>
+        <v>0.57</v>
       </c>
       <c r="F258" t="n">
         <v>371.8</v>
@@ -5614,7 +5614,7 @@
         <v>2001.458</v>
       </c>
       <c r="E259" t="n">
-        <v>0.58</v>
+        <v>0.53</v>
       </c>
       <c r="F259" t="n">
         <v>370.85</v>
@@ -5634,7 +5634,7 @@
         <v>2001.542</v>
       </c>
       <c r="E260" t="n">
-        <v>0.64</v>
+        <v>0.62</v>
       </c>
       <c r="F260" t="n">
         <v>369.46</v>
@@ -5654,7 +5654,7 @@
         <v>2001.625</v>
       </c>
       <c r="E261" t="n">
-        <v>0.5600000000000001</v>
+        <v>0.54</v>
       </c>
       <c r="F261" t="n">
         <v>368.32</v>
@@ -5674,7 +5674,7 @@
         <v>2001.708</v>
       </c>
       <c r="E262" t="n">
-        <v>0.61</v>
+        <v>0.55</v>
       </c>
       <c r="F262" t="n">
         <v>368.36</v>
@@ -5694,7 +5694,7 @@
         <v>2001.792</v>
       </c>
       <c r="E263" t="n">
-        <v>0.57</v>
+        <v>0.49</v>
       </c>
       <c r="F263" t="n">
         <v>369.71</v>
@@ -5714,7 +5714,7 @@
         <v>2001.875</v>
       </c>
       <c r="E264" t="n">
-        <v>0.57</v>
+        <v>0.68</v>
       </c>
       <c r="F264" t="n">
         <v>371.05</v>
@@ -5734,7 +5734,7 @@
         <v>2001.958</v>
       </c>
       <c r="E265" t="n">
-        <v>0.51</v>
+        <v>0.62</v>
       </c>
       <c r="F265" t="n">
         <v>371.97</v>
@@ -5754,7 +5754,7 @@
         <v>2002.042</v>
       </c>
       <c r="E266" t="n">
-        <v>0.72</v>
+        <v>0.68</v>
       </c>
       <c r="F266" t="n">
         <v>372.51</v>
@@ -5774,7 +5774,7 @@
         <v>2002.125</v>
       </c>
       <c r="E267" t="n">
-        <v>0.62</v>
+        <v>0.68</v>
       </c>
       <c r="F267" t="n">
         <v>372.91</v>
@@ -5794,7 +5794,7 @@
         <v>2002.208</v>
       </c>
       <c r="E268" t="n">
-        <v>0.59</v>
+        <v>0.83</v>
       </c>
       <c r="F268" t="n">
         <v>373.38</v>
@@ -5814,7 +5814,7 @@
         <v>2002.292</v>
       </c>
       <c r="E269" t="n">
-        <v>0.57</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="F269" t="n">
         <v>373.72</v>
@@ -5834,7 +5834,7 @@
         <v>2002.375</v>
       </c>
       <c r="E270" t="n">
-        <v>0.6</v>
+        <v>0.65</v>
       </c>
       <c r="F270" t="n">
         <v>373.71</v>
@@ -5854,7 +5854,7 @@
         <v>2002.458</v>
       </c>
       <c r="E271" t="n">
-        <v>0.49</v>
+        <v>0.58</v>
       </c>
       <c r="F271" t="n">
         <v>372.84</v>
@@ -5874,7 +5874,7 @@
         <v>2002.542</v>
       </c>
       <c r="E272" t="n">
-        <v>0.57</v>
+        <v>0.64</v>
       </c>
       <c r="F272" t="n">
         <v>371.41</v>
@@ -5894,7 +5894,7 @@
         <v>2002.625</v>
       </c>
       <c r="E273" t="n">
-        <v>0.64</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="F273" t="n">
         <v>370.37</v>
@@ -5914,7 +5914,7 @@
         <v>2002.708</v>
       </c>
       <c r="E274" t="n">
-        <v>0.68</v>
+        <v>0.61</v>
       </c>
       <c r="F274" t="n">
         <v>370.69</v>
@@ -5934,7 +5934,7 @@
         <v>2002.792</v>
       </c>
       <c r="E275" t="n">
-        <v>0.74</v>
+        <v>0.57</v>
       </c>
       <c r="F275" t="n">
         <v>371.96</v>
@@ -5954,7 +5954,7 @@
         <v>2002.875</v>
       </c>
       <c r="E276" t="n">
-        <v>0.5600000000000001</v>
+        <v>0.57</v>
       </c>
       <c r="F276" t="n">
         <v>373.29</v>
@@ -5974,7 +5974,7 @@
         <v>2002.958</v>
       </c>
       <c r="E277" t="n">
-        <v>0.74</v>
+        <v>0.51</v>
       </c>
       <c r="F277" t="n">
         <v>374.26</v>
@@ -5994,7 +5994,7 @@
         <v>2003.042</v>
       </c>
       <c r="E278" t="n">
-        <v>0.62</v>
+        <v>0.72</v>
       </c>
       <c r="F278" t="n">
         <v>374.94</v>
@@ -6014,7 +6014,7 @@
         <v>2003.125</v>
       </c>
       <c r="E279" t="n">
-        <v>0.71</v>
+        <v>0.62</v>
       </c>
       <c r="F279" t="n">
         <v>375.47</v>
@@ -6034,7 +6034,7 @@
         <v>2003.208</v>
       </c>
       <c r="E280" t="n">
-        <v>0.67</v>
+        <v>0.59</v>
       </c>
       <c r="F280" t="n">
         <v>375.92</v>
@@ -6054,7 +6054,7 @@
         <v>2003.292</v>
       </c>
       <c r="E281" t="n">
-        <v>0.61</v>
+        <v>0.57</v>
       </c>
       <c r="F281" t="n">
         <v>376.4</v>
@@ -6074,7 +6074,7 @@
         <v>2003.375</v>
       </c>
       <c r="E282" t="n">
-        <v>0.39</v>
+        <v>0.6</v>
       </c>
       <c r="F282" t="n">
         <v>376.55</v>
@@ -6094,7 +6094,7 @@
         <v>2003.458</v>
       </c>
       <c r="E283" t="n">
-        <v>0.44</v>
+        <v>0.49</v>
       </c>
       <c r="F283" t="n">
         <v>375.72</v>
@@ -6114,7 +6114,7 @@
         <v>2003.542</v>
       </c>
       <c r="E284" t="n">
-        <v>0.36</v>
+        <v>0.57</v>
       </c>
       <c r="F284" t="n">
         <v>374.17</v>
@@ -6134,7 +6134,7 @@
         <v>2003.625</v>
       </c>
       <c r="E285" t="n">
-        <v>0.49</v>
+        <v>0.64</v>
       </c>
       <c r="F285" t="n">
         <v>372.94</v>
@@ -6154,7 +6154,7 @@
         <v>2003.708</v>
       </c>
       <c r="E286" t="n">
-        <v>0.55</v>
+        <v>0.68</v>
       </c>
       <c r="F286" t="n">
         <v>373.11</v>
@@ -6174,7 +6174,7 @@
         <v>2003.792</v>
       </c>
       <c r="E287" t="n">
-        <v>0.62</v>
+        <v>0.74</v>
       </c>
       <c r="F287" t="n">
         <v>374.39</v>
@@ -6194,7 +6194,7 @@
         <v>2003.875</v>
       </c>
       <c r="E288" t="n">
-        <v>0.7</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="F288" t="n">
         <v>375.67</v>
@@ -6214,7 +6214,7 @@
         <v>2003.958</v>
       </c>
       <c r="E289" t="n">
-        <v>0.53</v>
+        <v>0.74</v>
       </c>
       <c r="F289" t="n">
         <v>376.53</v>
@@ -6234,7 +6234,7 @@
         <v>2004.042</v>
       </c>
       <c r="E290" t="n">
-        <v>0.76</v>
+        <v>0.62</v>
       </c>
       <c r="F290" t="n">
         <v>377.21</v>
@@ -6254,7 +6254,7 @@
         <v>2004.125</v>
       </c>
       <c r="E291" t="n">
-        <v>0.63</v>
+        <v>0.71</v>
       </c>
       <c r="F291" t="n">
         <v>377.73</v>
@@ -6274,7 +6274,7 @@
         <v>2004.208</v>
       </c>
       <c r="E292" t="n">
-        <v>0.75</v>
+        <v>0.67</v>
       </c>
       <c r="F292" t="n">
         <v>378.16</v>
@@ -6294,7 +6294,7 @@
         <v>2004.292</v>
       </c>
       <c r="E293" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.61</v>
       </c>
       <c r="F293" t="n">
         <v>378.48</v>
@@ -6314,7 +6314,7 @@
         <v>2004.375</v>
       </c>
       <c r="E294" t="n">
-        <v>0.66</v>
+        <v>0.39</v>
       </c>
       <c r="F294" t="n">
         <v>378.4</v>
@@ -6334,7 +6334,7 @@
         <v>2004.458</v>
       </c>
       <c r="E295" t="n">
-        <v>0.67</v>
+        <v>0.44</v>
       </c>
       <c r="F295" t="n">
         <v>377.51</v>
@@ -6354,7 +6354,7 @@
         <v>2004.542</v>
       </c>
       <c r="E296" t="n">
-        <v>0.64</v>
+        <v>0.36</v>
       </c>
       <c r="F296" t="n">
         <v>375.96</v>
@@ -6374,7 +6374,7 @@
         <v>2004.625</v>
       </c>
       <c r="E297" t="n">
-        <v>0.6</v>
+        <v>0.49</v>
       </c>
       <c r="F297" t="n">
         <v>374.49</v>
@@ -6394,7 +6394,7 @@
         <v>2004.708</v>
       </c>
       <c r="E298" t="n">
-        <v>0.7</v>
+        <v>0.55</v>
       </c>
       <c r="F298" t="n">
         <v>374.39</v>
@@ -6414,7 +6414,7 @@
         <v>2004.792</v>
       </c>
       <c r="E299" t="n">
-        <v>0.73</v>
+        <v>0.62</v>
       </c>
       <c r="F299" t="n">
         <v>375.73</v>
@@ -6434,7 +6434,7 @@
         <v>2004.875</v>
       </c>
       <c r="E300" t="n">
-        <v>0.77</v>
+        <v>0.7</v>
       </c>
       <c r="F300" t="n">
         <v>377.2</v>
@@ -6454,7 +6454,7 @@
         <v>2004.958</v>
       </c>
       <c r="E301" t="n">
-        <v>0.72</v>
+        <v>0.53</v>
       </c>
       <c r="F301" t="n">
         <v>378.17</v>
@@ -6474,7 +6474,7 @@
         <v>2005.042</v>
       </c>
       <c r="E302" t="n">
-        <v>0.6</v>
+        <v>0.76</v>
       </c>
       <c r="F302" t="n">
         <v>378.73</v>
@@ -6494,7 +6494,7 @@
         <v>2005.125</v>
       </c>
       <c r="E303" t="n">
-        <v>0.76</v>
+        <v>0.63</v>
       </c>
       <c r="F303" t="n">
         <v>379.27</v>
@@ -6514,7 +6514,7 @@
         <v>2005.208</v>
       </c>
       <c r="E304" t="n">
-        <v>0.66</v>
+        <v>0.75</v>
       </c>
       <c r="F304" t="n">
         <v>379.87</v>
@@ -6534,7 +6534,7 @@
         <v>2005.292</v>
       </c>
       <c r="E305" t="n">
-        <v>0.55</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="F305" t="n">
         <v>380.32</v>
@@ -6554,7 +6554,7 @@
         <v>2005.375</v>
       </c>
       <c r="E306" t="n">
-        <v>0.55</v>
+        <v>0.66</v>
       </c>
       <c r="F306" t="n">
         <v>380.42</v>
@@ -6574,7 +6574,7 @@
         <v>2005.458</v>
       </c>
       <c r="E307" t="n">
-        <v>0.64</v>
+        <v>0.67</v>
       </c>
       <c r="F307" t="n">
         <v>379.6</v>
@@ -6594,7 +6594,7 @@
         <v>2005.542</v>
       </c>
       <c r="E308" t="n">
-        <v>0.5600000000000001</v>
+        <v>0.64</v>
       </c>
       <c r="F308" t="n">
         <v>377.94</v>
@@ -6614,7 +6614,7 @@
         <v>2005.625</v>
       </c>
       <c r="E309" t="n">
-        <v>0.71</v>
+        <v>0.6</v>
       </c>
       <c r="F309" t="n">
         <v>376.73</v>
@@ -6634,7 +6634,7 @@
         <v>2005.708</v>
       </c>
       <c r="E310" t="n">
-        <v>0.67</v>
+        <v>0.7</v>
       </c>
       <c r="F310" t="n">
         <v>376.76</v>
@@ -6654,7 +6654,7 @@
         <v>2005.792</v>
       </c>
       <c r="E311" t="n">
-        <v>0.68</v>
+        <v>0.73</v>
       </c>
       <c r="F311" t="n">
         <v>378.07</v>
@@ -6674,7 +6674,7 @@
         <v>2005.875</v>
       </c>
       <c r="E312" t="n">
-        <v>0.68</v>
+        <v>0.77</v>
       </c>
       <c r="F312" t="n">
         <v>379.53</v>
@@ -6694,7 +6694,7 @@
         <v>2005.958</v>
       </c>
       <c r="E313" t="n">
-        <v>0.78</v>
+        <v>0.72</v>
       </c>
       <c r="F313" t="n">
         <v>380.53</v>
@@ -6714,7 +6714,7 @@
         <v>2006.042</v>
       </c>
       <c r="E314" t="n">
-        <v>0.92</v>
+        <v>0.6</v>
       </c>
       <c r="F314" t="n">
         <v>381.33</v>
@@ -6734,7 +6734,7 @@
         <v>2006.125</v>
       </c>
       <c r="E315" t="n">
-        <v>0.71</v>
+        <v>0.76</v>
       </c>
       <c r="F315" t="n">
         <v>381.95</v>
@@ -6754,7 +6754,7 @@
         <v>2006.208</v>
       </c>
       <c r="E316" t="n">
-        <v>0.68</v>
+        <v>0.66</v>
       </c>
       <c r="F316" t="n">
         <v>382.34</v>
@@ -6774,7 +6774,7 @@
         <v>2006.292</v>
       </c>
       <c r="E317" t="n">
-        <v>0.78</v>
+        <v>0.55</v>
       </c>
       <c r="F317" t="n">
         <v>382.67</v>
@@ -6794,7 +6794,7 @@
         <v>2006.375</v>
       </c>
       <c r="E318" t="n">
-        <v>0.64</v>
+        <v>0.55</v>
       </c>
       <c r="F318" t="n">
         <v>382.63</v>
@@ -6814,7 +6814,7 @@
         <v>2006.458</v>
       </c>
       <c r="E319" t="n">
-        <v>0.59</v>
+        <v>0.64</v>
       </c>
       <c r="F319" t="n">
         <v>381.76</v>
@@ -6834,7 +6834,7 @@
         <v>2006.542</v>
       </c>
       <c r="E320" t="n">
-        <v>0.59</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="F320" t="n">
         <v>380.07</v>
@@ -6854,7 +6854,7 @@
         <v>2006.625</v>
       </c>
       <c r="E321" t="n">
-        <v>0.57</v>
+        <v>0.71</v>
       </c>
       <c r="F321" t="n">
         <v>378.49</v>
@@ -6874,7 +6874,7 @@
         <v>2006.708</v>
       </c>
       <c r="E322" t="n">
-        <v>0.6</v>
+        <v>0.67</v>
       </c>
       <c r="F322" t="n">
         <v>378.63</v>
@@ -6894,7 +6894,7 @@
         <v>2006.792</v>
       </c>
       <c r="E323" t="n">
-        <v>0.6</v>
+        <v>0.68</v>
       </c>
       <c r="F323" t="n">
         <v>380.08</v>
@@ -6914,7 +6914,7 @@
         <v>2006.875</v>
       </c>
       <c r="E324" t="n">
-        <v>0.57</v>
+        <v>0.68</v>
       </c>
       <c r="F324" t="n">
         <v>381.44</v>
@@ -6934,7 +6934,7 @@
         <v>2006.958</v>
       </c>
       <c r="E325" t="n">
-        <v>0.48</v>
+        <v>0.78</v>
       </c>
       <c r="F325" t="n">
         <v>382.39</v>
@@ -6954,7 +6954,7 @@
         <v>2007.042</v>
       </c>
       <c r="E326" t="n">
-        <v>0.28</v>
+        <v>0.92</v>
       </c>
       <c r="F326" t="n">
         <v>383.03</v>
@@ -6974,7 +6974,7 @@
         <v>2007.125</v>
       </c>
       <c r="E327" t="n">
-        <v>0.32</v>
+        <v>0.71</v>
       </c>
       <c r="F327" t="n">
         <v>383.55</v>
@@ -6994,7 +6994,7 @@
         <v>2007.208</v>
       </c>
       <c r="E328" t="n">
-        <v>0.7</v>
+        <v>0.68</v>
       </c>
       <c r="F328" t="n">
         <v>384.02</v>
@@ -7014,7 +7014,7 @@
         <v>2007.292</v>
       </c>
       <c r="E329" t="n">
-        <v>0.52</v>
+        <v>0.78</v>
       </c>
       <c r="F329" t="n">
         <v>384.28</v>
@@ -7034,7 +7034,7 @@
         <v>2007.375</v>
       </c>
       <c r="E330" t="n">
-        <v>0.51</v>
+        <v>0.64</v>
       </c>
       <c r="F330" t="n">
         <v>384.13</v>
@@ -7054,7 +7054,7 @@
         <v>2007.458</v>
       </c>
       <c r="E331" t="n">
-        <v>0.48</v>
+        <v>0.59</v>
       </c>
       <c r="F331" t="n">
         <v>383.26</v>
@@ -7094,7 +7094,7 @@
         <v>2007.625</v>
       </c>
       <c r="E333" t="n">
-        <v>0.53</v>
+        <v>0.57</v>
       </c>
       <c r="F333" t="n">
         <v>380.29</v>
@@ -7114,7 +7114,7 @@
         <v>2007.708</v>
       </c>
       <c r="E334" t="n">
-        <v>0.61</v>
+        <v>0.6</v>
       </c>
       <c r="F334" t="n">
         <v>380.68</v>
@@ -7134,7 +7134,7 @@
         <v>2007.792</v>
       </c>
       <c r="E335" t="n">
-        <v>0.68</v>
+        <v>0.6</v>
       </c>
       <c r="F335" t="n">
         <v>382.1</v>
@@ -7154,7 +7154,7 @@
         <v>2007.875</v>
       </c>
       <c r="E336" t="n">
-        <v>0.7</v>
+        <v>0.57</v>
       </c>
       <c r="F336" t="n">
         <v>383.45</v>
@@ -7174,7 +7174,7 @@
         <v>2007.958</v>
       </c>
       <c r="E337" t="n">
-        <v>0.59</v>
+        <v>0.48</v>
       </c>
       <c r="F337" t="n">
         <v>384.46</v>
@@ -7194,7 +7194,7 @@
         <v>2008.042</v>
       </c>
       <c r="E338" t="n">
-        <v>0.67</v>
+        <v>0.28</v>
       </c>
       <c r="F338" t="n">
         <v>385.23</v>
@@ -7214,7 +7214,7 @@
         <v>2008.125</v>
       </c>
       <c r="E339" t="n">
-        <v>0.54</v>
+        <v>0.32</v>
       </c>
       <c r="F339" t="n">
         <v>385.74</v>
@@ -7234,7 +7234,7 @@
         <v>2008.208</v>
       </c>
       <c r="E340" t="n">
-        <v>0.53</v>
+        <v>0.7</v>
       </c>
       <c r="F340" t="n">
         <v>386.15</v>
@@ -7254,7 +7254,7 @@
         <v>2008.292</v>
       </c>
       <c r="E341" t="n">
-        <v>0.58</v>
+        <v>0.52</v>
       </c>
       <c r="F341" t="n">
         <v>386.53</v>
@@ -7274,7 +7274,7 @@
         <v>2008.375</v>
       </c>
       <c r="E342" t="n">
-        <v>0.62</v>
+        <v>0.51</v>
       </c>
       <c r="F342" t="n">
         <v>386.49</v>
@@ -7294,7 +7294,7 @@
         <v>2008.458</v>
       </c>
       <c r="E343" t="n">
-        <v>0.67</v>
+        <v>0.48</v>
       </c>
       <c r="F343" t="n">
         <v>385.58</v>
@@ -7314,7 +7314,7 @@
         <v>2008.542</v>
       </c>
       <c r="E344" t="n">
-        <v>0.74</v>
+        <v>0.59</v>
       </c>
       <c r="F344" t="n">
         <v>384.1</v>
@@ -7334,7 +7334,7 @@
         <v>2008.625</v>
       </c>
       <c r="E345" t="n">
-        <v>0.71</v>
+        <v>0.53</v>
       </c>
       <c r="F345" t="n">
         <v>382.77</v>
@@ -7354,7 +7354,7 @@
         <v>2008.708</v>
       </c>
       <c r="E346" t="n">
-        <v>0.76</v>
+        <v>0.61</v>
       </c>
       <c r="F346" t="n">
         <v>382.54</v>
@@ -7374,7 +7374,7 @@
         <v>2008.792</v>
       </c>
       <c r="E347" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.68</v>
       </c>
       <c r="F347" t="n">
         <v>383.67</v>
@@ -7394,7 +7394,7 @@
         <v>2008.875</v>
       </c>
       <c r="E348" t="n">
-        <v>0.76</v>
+        <v>0.7</v>
       </c>
       <c r="F348" t="n">
         <v>385.18</v>
@@ -7414,7 +7414,7 @@
         <v>2008.958</v>
       </c>
       <c r="E349" t="n">
-        <v>0.72</v>
+        <v>0.59</v>
       </c>
       <c r="F349" t="n">
         <v>386.27</v>
@@ -7434,7 +7434,7 @@
         <v>2009.042</v>
       </c>
       <c r="E350" t="n">
-        <v>0.77</v>
+        <v>0.67</v>
       </c>
       <c r="F350" t="n">
         <v>387.03</v>
@@ -7454,7 +7454,7 @@
         <v>2009.125</v>
       </c>
       <c r="E351" t="n">
-        <v>0.84</v>
+        <v>0.54</v>
       </c>
       <c r="F351" t="n">
         <v>387.48</v>
@@ -7474,7 +7474,7 @@
         <v>2009.208</v>
       </c>
       <c r="E352" t="n">
-        <v>0.89</v>
+        <v>0.53</v>
       </c>
       <c r="F352" t="n">
         <v>387.71</v>
@@ -7494,7 +7494,7 @@
         <v>2009.292</v>
       </c>
       <c r="E353" t="n">
-        <v>0.88</v>
+        <v>0.58</v>
       </c>
       <c r="F353" t="n">
         <v>387.99</v>
@@ -7514,7 +7514,7 @@
         <v>2009.375</v>
       </c>
       <c r="E354" t="n">
-        <v>0.78</v>
+        <v>0.62</v>
       </c>
       <c r="F354" t="n">
         <v>387.95</v>
@@ -7534,7 +7534,7 @@
         <v>2009.458</v>
       </c>
       <c r="E355" t="n">
-        <v>0.7</v>
+        <v>0.67</v>
       </c>
       <c r="F355" t="n">
         <v>386.96</v>
@@ -7554,7 +7554,7 @@
         <v>2009.542</v>
       </c>
       <c r="E356" t="n">
-        <v>0.67</v>
+        <v>0.74</v>
       </c>
       <c r="F356" t="n">
         <v>385.01</v>
@@ -7574,7 +7574,7 @@
         <v>2009.625</v>
       </c>
       <c r="E357" t="n">
-        <v>0.65</v>
+        <v>0.71</v>
       </c>
       <c r="F357" t="n">
         <v>383.63</v>
@@ -7594,7 +7594,7 @@
         <v>2009.708</v>
       </c>
       <c r="E358" t="n">
-        <v>0.65</v>
+        <v>0.76</v>
       </c>
       <c r="F358" t="n">
         <v>383.93</v>
@@ -7614,7 +7614,7 @@
         <v>2009.792</v>
       </c>
       <c r="E359" t="n">
-        <v>0.68</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="F359" t="n">
         <v>385.5</v>
@@ -7634,7 +7634,7 @@
         <v>2009.875</v>
       </c>
       <c r="E360" t="n">
-        <v>0.77</v>
+        <v>0.76</v>
       </c>
       <c r="F360" t="n">
         <v>386.94</v>
@@ -7654,7 +7654,7 @@
         <v>2009.958</v>
       </c>
       <c r="E361" t="n">
-        <v>0.51</v>
+        <v>0.72</v>
       </c>
       <c r="F361" t="n">
         <v>387.84</v>
@@ -7674,7 +7674,7 @@
         <v>2010.042</v>
       </c>
       <c r="E362" t="n">
-        <v>0.5600000000000001</v>
+        <v>0.77</v>
       </c>
       <c r="F362" t="n">
         <v>388.62</v>
@@ -7694,7 +7694,7 @@
         <v>2010.125</v>
       </c>
       <c r="E363" t="n">
-        <v>0.51</v>
+        <v>0.84</v>
       </c>
       <c r="F363" t="n">
         <v>389.33</v>
@@ -7714,7 +7714,7 @@
         <v>2010.208</v>
       </c>
       <c r="E364" t="n">
-        <v>0.65</v>
+        <v>0.89</v>
       </c>
       <c r="F364" t="n">
         <v>389.68</v>
@@ -7734,7 +7734,7 @@
         <v>2010.292</v>
       </c>
       <c r="E365" t="n">
-        <v>0.66</v>
+        <v>0.88</v>
       </c>
       <c r="F365" t="n">
         <v>389.98</v>
@@ -7754,7 +7754,7 @@
         <v>2010.375</v>
       </c>
       <c r="E366" t="n">
-        <v>0.55</v>
+        <v>0.78</v>
       </c>
       <c r="F366" t="n">
         <v>389.95</v>
@@ -7774,7 +7774,7 @@
         <v>2010.458</v>
       </c>
       <c r="E367" t="n">
-        <v>0.62</v>
+        <v>0.7</v>
       </c>
       <c r="F367" t="n">
         <v>389.01</v>
@@ -7794,7 +7794,7 @@
         <v>2010.542</v>
       </c>
       <c r="E368" t="n">
-        <v>0.7</v>
+        <v>0.67</v>
       </c>
       <c r="F368" t="n">
         <v>387.35</v>
@@ -7814,7 +7814,7 @@
         <v>2010.625</v>
       </c>
       <c r="E369" t="n">
-        <v>0.7</v>
+        <v>0.65</v>
       </c>
       <c r="F369" t="n">
         <v>386.23</v>
@@ -7834,7 +7834,7 @@
         <v>2010.708</v>
       </c>
       <c r="E370" t="n">
-        <v>0.62</v>
+        <v>0.65</v>
       </c>
       <c r="F370" t="n">
         <v>386.7</v>
@@ -7854,7 +7854,7 @@
         <v>2010.792</v>
       </c>
       <c r="E371" t="n">
-        <v>0.66</v>
+        <v>0.68</v>
       </c>
       <c r="F371" t="n">
         <v>388.25</v>
@@ -7874,7 +7874,7 @@
         <v>2010.875</v>
       </c>
       <c r="E372" t="n">
-        <v>0.55</v>
+        <v>0.77</v>
       </c>
       <c r="F372" t="n">
         <v>389.62</v>
@@ -7894,7 +7894,7 @@
         <v>2010.958</v>
       </c>
       <c r="E373" t="n">
-        <v>0.59</v>
+        <v>0.51</v>
       </c>
       <c r="F373" t="n">
         <v>390.36</v>
@@ -7914,7 +7914,7 @@
         <v>2011.042</v>
       </c>
       <c r="E374" t="n">
-        <v>0.51</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="F374" t="n">
         <v>390.93</v>
@@ -7934,7 +7934,7 @@
         <v>2011.125</v>
       </c>
       <c r="E375" t="n">
-        <v>0.52</v>
+        <v>0.51</v>
       </c>
       <c r="F375" t="n">
         <v>391.35</v>
@@ -7954,7 +7954,7 @@
         <v>2011.208</v>
       </c>
       <c r="E376" t="n">
-        <v>0.53</v>
+        <v>0.65</v>
       </c>
       <c r="F376" t="n">
         <v>391.67</v>
@@ -7974,7 +7974,7 @@
         <v>2011.292</v>
       </c>
       <c r="E377" t="n">
-        <v>0.72</v>
+        <v>0.66</v>
       </c>
       <c r="F377" t="n">
         <v>392.05</v>
@@ -7994,7 +7994,7 @@
         <v>2011.375</v>
       </c>
       <c r="E378" t="n">
-        <v>0.75</v>
+        <v>0.55</v>
       </c>
       <c r="F378" t="n">
         <v>392.07</v>
@@ -8014,7 +8014,7 @@
         <v>2011.458</v>
       </c>
       <c r="E379" t="n">
-        <v>0.7</v>
+        <v>0.62</v>
       </c>
       <c r="F379" t="n">
         <v>391.13</v>
@@ -8034,7 +8034,7 @@
         <v>2011.542</v>
       </c>
       <c r="E380" t="n">
-        <v>0.63</v>
+        <v>0.7</v>
       </c>
       <c r="F380" t="n">
         <v>389.19</v>
@@ -8054,7 +8054,7 @@
         <v>2011.625</v>
       </c>
       <c r="E381" t="n">
-        <v>0.67</v>
+        <v>0.7</v>
       </c>
       <c r="F381" t="n">
         <v>387.86</v>
@@ -8074,7 +8074,7 @@
         <v>2011.708</v>
       </c>
       <c r="E382" t="n">
-        <v>0.74</v>
+        <v>0.62</v>
       </c>
       <c r="F382" t="n">
         <v>388.26</v>
@@ -8094,7 +8094,7 @@
         <v>2011.792</v>
       </c>
       <c r="E383" t="n">
-        <v>0.78</v>
+        <v>0.66</v>
       </c>
       <c r="F383" t="n">
         <v>389.83</v>
@@ -8114,7 +8114,7 @@
         <v>2011.875</v>
       </c>
       <c r="E384" t="n">
-        <v>0.75</v>
+        <v>0.55</v>
       </c>
       <c r="F384" t="n">
         <v>391.2</v>
@@ -8134,7 +8134,7 @@
         <v>2011.958</v>
       </c>
       <c r="E385" t="n">
-        <v>0.53</v>
+        <v>0.59</v>
       </c>
       <c r="F385" t="n">
         <v>392.04</v>
@@ -8154,7 +8154,7 @@
         <v>2012.042</v>
       </c>
       <c r="E386" t="n">
-        <v>0.68</v>
+        <v>0.51</v>
       </c>
       <c r="F386" t="n">
         <v>392.61</v>
@@ -8174,7 +8174,7 @@
         <v>2012.125</v>
       </c>
       <c r="E387" t="n">
-        <v>0.6</v>
+        <v>0.52</v>
       </c>
       <c r="F387" t="n">
         <v>393.2</v>
@@ -8194,7 +8194,7 @@
         <v>2012.208</v>
       </c>
       <c r="E388" t="n">
-        <v>0.66</v>
+        <v>0.53</v>
       </c>
       <c r="F388" t="n">
         <v>393.73</v>
@@ -8214,7 +8214,7 @@
         <v>2012.292</v>
       </c>
       <c r="E389" t="n">
-        <v>0.6</v>
+        <v>0.72</v>
       </c>
       <c r="F389" t="n">
         <v>393.99</v>
@@ -8234,7 +8234,7 @@
         <v>2012.375</v>
       </c>
       <c r="E390" t="n">
-        <v>0.66</v>
+        <v>0.75</v>
       </c>
       <c r="F390" t="n">
         <v>393.88</v>
@@ -8274,7 +8274,7 @@
         <v>2012.542</v>
       </c>
       <c r="E392" t="n">
-        <v>0.62</v>
+        <v>0.63</v>
       </c>
       <c r="F392" t="n">
         <v>391</v>
@@ -8294,7 +8294,7 @@
         <v>2012.625</v>
       </c>
       <c r="E393" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.67</v>
       </c>
       <c r="F393" t="n">
         <v>389.89</v>
@@ -8314,7 +8314,7 @@
         <v>2012.708</v>
       </c>
       <c r="E394" t="n">
-        <v>0.76</v>
+        <v>0.74</v>
       </c>
       <c r="F394" t="n">
         <v>390.55</v>
@@ -8334,7 +8334,7 @@
         <v>2012.792</v>
       </c>
       <c r="E395" t="n">
-        <v>0.68</v>
+        <v>0.78</v>
       </c>
       <c r="F395" t="n">
         <v>392.16</v>
@@ -8354,7 +8354,7 @@
         <v>2012.875</v>
       </c>
       <c r="E396" t="n">
-        <v>0.79</v>
+        <v>0.75</v>
       </c>
       <c r="F396" t="n">
         <v>393.56</v>
@@ -8374,7 +8374,7 @@
         <v>2012.958</v>
       </c>
       <c r="E397" t="n">
-        <v>0.7</v>
+        <v>0.53</v>
       </c>
       <c r="F397" t="n">
         <v>394.39</v>
@@ -8394,7 +8394,7 @@
         <v>2013.042</v>
       </c>
       <c r="E398" t="n">
-        <v>0.75</v>
+        <v>0.68</v>
       </c>
       <c r="F398" t="n">
         <v>395.07</v>
@@ -8414,7 +8414,7 @@
         <v>2013.125</v>
       </c>
       <c r="E399" t="n">
-        <v>0.59</v>
+        <v>0.6</v>
       </c>
       <c r="F399" t="n">
         <v>395.7</v>
@@ -8434,7 +8434,7 @@
         <v>2013.208</v>
       </c>
       <c r="E400" t="n">
-        <v>0.79</v>
+        <v>0.66</v>
       </c>
       <c r="F400" t="n">
         <v>396.29</v>
@@ -8454,7 +8454,7 @@
         <v>2013.292</v>
       </c>
       <c r="E401" t="n">
-        <v>0.79</v>
+        <v>0.6</v>
       </c>
       <c r="F401" t="n">
         <v>396.74</v>
@@ -8474,7 +8474,7 @@
         <v>2013.375</v>
       </c>
       <c r="E402" t="n">
-        <v>0.83</v>
+        <v>0.66</v>
       </c>
       <c r="F402" t="n">
         <v>396.75</v>
@@ -8494,7 +8494,7 @@
         <v>2013.458</v>
       </c>
       <c r="E403" t="n">
-        <v>0.72</v>
+        <v>0.7</v>
       </c>
       <c r="F403" t="n">
         <v>395.96</v>
@@ -8514,7 +8514,7 @@
         <v>2013.542</v>
       </c>
       <c r="E404" t="n">
-        <v>0.65</v>
+        <v>0.62</v>
       </c>
       <c r="F404" t="n">
         <v>394.47</v>
@@ -8534,7 +8534,7 @@
         <v>2013.625</v>
       </c>
       <c r="E405" t="n">
-        <v>0.82</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="F405" t="n">
         <v>393.24</v>
@@ -8554,7 +8554,7 @@
         <v>2013.708</v>
       </c>
       <c r="E406" t="n">
-        <v>0.84</v>
+        <v>0.76</v>
       </c>
       <c r="F406" t="n">
         <v>393.21</v>
@@ -8574,7 +8574,7 @@
         <v>2013.792</v>
       </c>
       <c r="E407" t="n">
-        <v>0.78</v>
+        <v>0.68</v>
       </c>
       <c r="F407" t="n">
         <v>394.51</v>
@@ -8594,7 +8594,7 @@
         <v>2013.875</v>
       </c>
       <c r="E408" t="n">
-        <v>0.67</v>
+        <v>0.79</v>
       </c>
       <c r="F408" t="n">
         <v>395.97</v>
@@ -8614,7 +8614,7 @@
         <v>2013.958</v>
       </c>
       <c r="E409" t="n">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="F409" t="n">
         <v>396.87</v>
@@ -8634,7 +8634,7 @@
         <v>2014.042</v>
       </c>
       <c r="E410" t="n">
-        <v>0.83</v>
+        <v>0.75</v>
       </c>
       <c r="F410" t="n">
         <v>397.51</v>
@@ -8654,7 +8654,7 @@
         <v>2014.125</v>
       </c>
       <c r="E411" t="n">
-        <v>0.87</v>
+        <v>0.59</v>
       </c>
       <c r="F411" t="n">
         <v>397.97</v>
@@ -8674,7 +8674,7 @@
         <v>2014.208</v>
       </c>
       <c r="E412" t="n">
-        <v>0.93</v>
+        <v>0.79</v>
       </c>
       <c r="F412" t="n">
         <v>398.27</v>
@@ -8694,7 +8694,7 @@
         <v>2014.292</v>
       </c>
       <c r="E413" t="n">
-        <v>0.8100000000000001</v>
+        <v>0.79</v>
       </c>
       <c r="F413" t="n">
         <v>398.63</v>
@@ -8714,7 +8714,7 @@
         <v>2014.375</v>
       </c>
       <c r="E414" t="n">
-        <v>0.82</v>
+        <v>0.83</v>
       </c>
       <c r="F414" t="n">
         <v>398.69</v>
@@ -8734,7 +8734,7 @@
         <v>2014.458</v>
       </c>
       <c r="E415" t="n">
-        <v>0.86</v>
+        <v>0.72</v>
       </c>
       <c r="F415" t="n">
         <v>397.72</v>
@@ -8754,7 +8754,7 @@
         <v>2014.542</v>
       </c>
       <c r="E416" t="n">
-        <v>0.79</v>
+        <v>0.65</v>
       </c>
       <c r="F416" t="n">
         <v>396.13</v>
@@ -8774,7 +8774,7 @@
         <v>2014.625</v>
       </c>
       <c r="E417" t="n">
-        <v>0.84</v>
+        <v>0.82</v>
       </c>
       <c r="F417" t="n">
         <v>395.02</v>
@@ -8794,7 +8794,7 @@
         <v>2014.708</v>
       </c>
       <c r="E418" t="n">
-        <v>0.93</v>
+        <v>0.84</v>
       </c>
       <c r="F418" t="n">
         <v>395.12</v>
@@ -8814,7 +8814,7 @@
         <v>2014.792</v>
       </c>
       <c r="E419" t="n">
-        <v>1.07</v>
+        <v>0.78</v>
       </c>
       <c r="F419" t="n">
         <v>396.38</v>
@@ -8834,7 +8834,7 @@
         <v>2014.875</v>
       </c>
       <c r="E420" t="n">
-        <v>1.04</v>
+        <v>0.67</v>
       </c>
       <c r="F420" t="n">
         <v>397.86</v>
@@ -8854,7 +8854,7 @@
         <v>2014.958</v>
       </c>
       <c r="E421" t="n">
-        <v>1.12</v>
+        <v>0.8</v>
       </c>
       <c r="F421" t="n">
         <v>398.84</v>
@@ -8874,7 +8874,7 @@
         <v>2015.042</v>
       </c>
       <c r="E422" t="n">
-        <v>1.21</v>
+        <v>0.83</v>
       </c>
       <c r="F422" t="n">
         <v>399.56</v>
@@ -8894,7 +8894,7 @@
         <v>2015.125</v>
       </c>
       <c r="E423" t="n">
-        <v>1.34</v>
+        <v>0.87</v>
       </c>
       <c r="F423" t="n">
         <v>400.12</v>
@@ -8914,7 +8914,7 @@
         <v>2015.208</v>
       </c>
       <c r="E424" t="n">
-        <v>1.33</v>
+        <v>0.93</v>
       </c>
       <c r="F424" t="n">
         <v>400.57</v>
@@ -8934,7 +8934,7 @@
         <v>2015.292</v>
       </c>
       <c r="E425" t="n">
-        <v>1.14</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="F425" t="n">
         <v>400.96</v>
@@ -8954,7 +8954,7 @@
         <v>2015.375</v>
       </c>
       <c r="E426" t="n">
-        <v>0.96</v>
+        <v>0.82</v>
       </c>
       <c r="F426" t="n">
         <v>400.91</v>
@@ -8974,7 +8974,7 @@
         <v>2015.458</v>
       </c>
       <c r="E427" t="n">
-        <v>0.84</v>
+        <v>0.86</v>
       </c>
       <c r="F427" t="n">
         <v>400.06</v>
@@ -8994,7 +8994,7 @@
         <v>2015.542</v>
       </c>
       <c r="E428" t="n">
-        <v>0.87</v>
+        <v>0.79</v>
       </c>
       <c r="F428" t="n">
         <v>398.38</v>
@@ -9014,7 +9014,7 @@
         <v>2015.625</v>
       </c>
       <c r="E429" t="n">
-        <v>1</v>
+        <v>0.84</v>
       </c>
       <c r="F429" t="n">
         <v>397.07</v>
@@ -9034,7 +9034,7 @@
         <v>2015.708</v>
       </c>
       <c r="E430" t="n">
-        <v>0.95</v>
+        <v>0.93</v>
       </c>
       <c r="F430" t="n">
         <v>397.34</v>
@@ -9054,7 +9054,7 @@
         <v>2015.792</v>
       </c>
       <c r="E431" t="n">
-        <v>0.87</v>
+        <v>1.07</v>
       </c>
       <c r="F431" t="n">
         <v>398.8</v>
@@ -9074,7 +9074,7 @@
         <v>2015.875</v>
       </c>
       <c r="E432" t="n">
-        <v>0.93</v>
+        <v>1.04</v>
       </c>
       <c r="F432" t="n">
         <v>400.36</v>
@@ -9094,7 +9094,7 @@
         <v>2015.958</v>
       </c>
       <c r="E433" t="n">
-        <v>0.9</v>
+        <v>1.12</v>
       </c>
       <c r="F433" t="n">
         <v>401.66</v>
@@ -9114,7 +9114,7 @@
         <v>2016.042</v>
       </c>
       <c r="E434" t="n">
-        <v>1.04</v>
+        <v>1.21</v>
       </c>
       <c r="F434" t="n">
         <v>402.61</v>
@@ -9134,7 +9134,7 @@
         <v>2016.125</v>
       </c>
       <c r="E435" t="n">
-        <v>1.1</v>
+        <v>1.34</v>
       </c>
       <c r="F435" t="n">
         <v>403.25</v>
@@ -9154,7 +9154,7 @@
         <v>2016.208</v>
       </c>
       <c r="E436" t="n">
-        <v>1.11</v>
+        <v>1.33</v>
       </c>
       <c r="F436" t="n">
         <v>403.84</v>
@@ -9174,7 +9174,7 @@
         <v>2016.292</v>
       </c>
       <c r="E437" t="n">
-        <v>0.95</v>
+        <v>1.14</v>
       </c>
       <c r="F437" t="n">
         <v>404.36</v>
@@ -9194,7 +9194,7 @@
         <v>2016.375</v>
       </c>
       <c r="E438" t="n">
-        <v>0.91</v>
+        <v>0.96</v>
       </c>
       <c r="F438" t="n">
         <v>404.4</v>
@@ -9214,7 +9214,7 @@
         <v>2016.458</v>
       </c>
       <c r="E439" t="n">
-        <v>0.77</v>
+        <v>0.84</v>
       </c>
       <c r="F439" t="n">
         <v>403.62</v>
@@ -9234,7 +9234,7 @@
         <v>2016.542</v>
       </c>
       <c r="E440" t="n">
-        <v>0.85</v>
+        <v>0.87</v>
       </c>
       <c r="F440" t="n">
         <v>402.1</v>
@@ -9254,7 +9254,7 @@
         <v>2016.625</v>
       </c>
       <c r="E441" t="n">
-        <v>0.87</v>
+        <v>1</v>
       </c>
       <c r="F441" t="n">
         <v>400.78</v>
@@ -9274,7 +9274,7 @@
         <v>2016.708</v>
       </c>
       <c r="E442" t="n">
-        <v>0.86</v>
+        <v>0.95</v>
       </c>
       <c r="F442" t="n">
         <v>400.95</v>
@@ -9294,7 +9294,7 @@
         <v>2016.792</v>
       </c>
       <c r="E443" t="n">
-        <v>0.91</v>
+        <v>0.87</v>
       </c>
       <c r="F443" t="n">
         <v>402.4</v>
@@ -9314,7 +9314,7 @@
         <v>2016.875</v>
       </c>
       <c r="E444" t="n">
-        <v>0.89</v>
+        <v>0.93</v>
       </c>
       <c r="F444" t="n">
         <v>403.76</v>
@@ -9334,7 +9334,7 @@
         <v>2016.958</v>
       </c>
       <c r="E445" t="n">
-        <v>0.96</v>
+        <v>0.9</v>
       </c>
       <c r="F445" t="n">
         <v>404.67</v>
@@ -9354,7 +9354,7 @@
         <v>2017.042</v>
       </c>
       <c r="E446" t="n">
-        <v>0.84</v>
+        <v>1.04</v>
       </c>
       <c r="F446" t="n">
         <v>405.33</v>
@@ -9374,7 +9374,7 @@
         <v>2017.125</v>
       </c>
       <c r="E447" t="n">
-        <v>0.88</v>
+        <v>1.1</v>
       </c>
       <c r="F447" t="n">
         <v>405.91</v>
@@ -9394,7 +9394,7 @@
         <v>2017.208</v>
       </c>
       <c r="E448" t="n">
-        <v>0.88</v>
+        <v>1.11</v>
       </c>
       <c r="F448" t="n">
         <v>406.32</v>
@@ -9414,7 +9414,7 @@
         <v>2017.292</v>
       </c>
       <c r="E449" t="n">
-        <v>0.9</v>
+        <v>0.95</v>
       </c>
       <c r="F449" t="n">
         <v>406.6</v>
@@ -9434,7 +9434,7 @@
         <v>2017.375</v>
       </c>
       <c r="E450" t="n">
-        <v>0.83</v>
+        <v>0.91</v>
       </c>
       <c r="F450" t="n">
         <v>406.64</v>
@@ -9454,7 +9454,7 @@
         <v>2017.458</v>
       </c>
       <c r="E451" t="n">
-        <v>0.79</v>
+        <v>0.77</v>
       </c>
       <c r="F451" t="n">
         <v>405.85</v>
@@ -9474,7 +9474,7 @@
         <v>2017.542</v>
       </c>
       <c r="E452" t="n">
-        <v>0.84</v>
+        <v>0.85</v>
       </c>
       <c r="F452" t="n">
         <v>404.11</v>
@@ -9494,7 +9494,7 @@
         <v>2017.625</v>
       </c>
       <c r="E453" t="n">
-        <v>0.8100000000000001</v>
+        <v>0.87</v>
       </c>
       <c r="F453" t="n">
         <v>402.57</v>
@@ -9514,7 +9514,7 @@
         <v>2017.708</v>
       </c>
       <c r="E454" t="n">
-        <v>0.82</v>
+        <v>0.86</v>
       </c>
       <c r="F454" t="n">
         <v>402.66</v>
@@ -9534,7 +9534,7 @@
         <v>2017.792</v>
       </c>
       <c r="E455" t="n">
-        <v>1.01</v>
+        <v>0.91</v>
       </c>
       <c r="F455" t="n">
         <v>404.16</v>
@@ -9554,7 +9554,7 @@
         <v>2017.875</v>
       </c>
       <c r="E456" t="n">
-        <v>0.84</v>
+        <v>0.89</v>
       </c>
       <c r="F456" t="n">
         <v>405.7</v>
@@ -9574,7 +9574,7 @@
         <v>2017.958</v>
       </c>
       <c r="E457" t="n">
-        <v>0.9399999999999999</v>
+        <v>0.96</v>
       </c>
       <c r="F457" t="n">
         <v>406.75</v>
@@ -9594,7 +9594,7 @@
         <v>2018.042</v>
       </c>
       <c r="E458" t="n">
-        <v>0.92</v>
+        <v>0.84</v>
       </c>
       <c r="F458" t="n">
         <v>407.53</v>
@@ -9614,7 +9614,7 @@
         <v>2018.125</v>
       </c>
       <c r="E459" t="n">
-        <v>0.91</v>
+        <v>0.88</v>
       </c>
       <c r="F459" t="n">
         <v>408.23</v>
@@ -9634,7 +9634,7 @@
         <v>2018.208</v>
       </c>
       <c r="E460" t="n">
-        <v>1.15</v>
+        <v>0.88</v>
       </c>
       <c r="F460" t="n">
         <v>408.77</v>
@@ -9654,7 +9654,7 @@
         <v>2018.292</v>
       </c>
       <c r="E461" t="n">
-        <v>1.04</v>
+        <v>0.9</v>
       </c>
       <c r="F461" t="n">
         <v>409.07</v>
@@ -9674,7 +9674,7 @@
         <v>2018.375</v>
       </c>
       <c r="E462" t="n">
-        <v>0.91</v>
+        <v>0.83</v>
       </c>
       <c r="F462" t="n">
         <v>408.93</v>
@@ -9694,7 +9694,7 @@
         <v>2018.458</v>
       </c>
       <c r="E463" t="n">
-        <v>0.91</v>
+        <v>0.79</v>
       </c>
       <c r="F463" t="n">
         <v>408.06</v>
@@ -9714,7 +9714,7 @@
         <v>2018.542</v>
       </c>
       <c r="E464" t="n">
-        <v>0.92</v>
+        <v>0.84</v>
       </c>
       <c r="F464" t="n">
         <v>406.49</v>
@@ -9734,7 +9734,7 @@
         <v>2018.625</v>
       </c>
       <c r="E465" t="n">
-        <v>0.93</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="F465" t="n">
         <v>405.11</v>
@@ -9754,7 +9754,7 @@
         <v>2018.708</v>
       </c>
       <c r="E466" t="n">
-        <v>0.9399999999999999</v>
+        <v>0.82</v>
       </c>
       <c r="F466" t="n">
         <v>405.18</v>
@@ -9774,7 +9774,7 @@
         <v>2018.792</v>
       </c>
       <c r="E467" t="n">
-        <v>1.02</v>
+        <v>1.01</v>
       </c>
       <c r="F467" t="n">
         <v>406.65</v>
@@ -9794,7 +9794,7 @@
         <v>2018.875</v>
       </c>
       <c r="E468" t="n">
-        <v>0.98</v>
+        <v>0.84</v>
       </c>
       <c r="F468" t="n">
         <v>408.12</v>
@@ -9814,7 +9814,7 @@
         <v>2018.958</v>
       </c>
       <c r="E469" t="n">
-        <v>1.11</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="F469" t="n">
         <v>409.19</v>
@@ -9834,7 +9834,7 @@
         <v>2019.042</v>
       </c>
       <c r="E470" t="n">
-        <v>1.16</v>
+        <v>0.92</v>
       </c>
       <c r="F470" t="n">
         <v>409.92</v>
@@ -9854,7 +9854,7 @@
         <v>2019.125</v>
       </c>
       <c r="E471" t="n">
-        <v>1.21</v>
+        <v>0.91</v>
       </c>
       <c r="F471" t="n">
         <v>410.34</v>
@@ -9874,7 +9874,7 @@
         <v>2019.208</v>
       </c>
       <c r="E472" t="n">
-        <v>1.14</v>
+        <v>1.15</v>
       </c>
       <c r="F472" t="n">
         <v>410.89</v>
@@ -9894,7 +9894,7 @@
         <v>2019.292</v>
       </c>
       <c r="E473" t="n">
-        <v>1.13</v>
+        <v>1.04</v>
       </c>
       <c r="F473" t="n">
         <v>411.33</v>
@@ -9914,7 +9914,7 @@
         <v>2019.375</v>
       </c>
       <c r="E474" t="n">
-        <v>0.99</v>
+        <v>0.91</v>
       </c>
       <c r="F474" t="n">
         <v>411.34</v>
@@ -9934,7 +9934,7 @@
         <v>2019.458</v>
       </c>
       <c r="E475" t="n">
-        <v>0.93</v>
+        <v>0.91</v>
       </c>
       <c r="F475" t="n">
         <v>410.53</v>
@@ -9954,7 +9954,7 @@
         <v>2019.542</v>
       </c>
       <c r="E476" t="n">
-        <v>0.91</v>
+        <v>0.92</v>
       </c>
       <c r="F476" t="n">
         <v>408.88</v>
@@ -9974,7 +9974,7 @@
         <v>2019.625</v>
       </c>
       <c r="E477" t="n">
-        <v>0.9</v>
+        <v>0.93</v>
       </c>
       <c r="F477" t="n">
         <v>407.64</v>
@@ -9994,7 +9994,7 @@
         <v>2019.708</v>
       </c>
       <c r="E478" t="n">
-        <v>1</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="F478" t="n">
         <v>407.92</v>
@@ -10014,7 +10014,7 @@
         <v>2019.792</v>
       </c>
       <c r="E479" t="n">
-        <v>0.9</v>
+        <v>1.02</v>
       </c>
       <c r="F479" t="n">
         <v>409.44</v>
@@ -10034,7 +10034,7 @@
         <v>2019.875</v>
       </c>
       <c r="E480" t="n">
-        <v>1.06</v>
+        <v>0.98</v>
       </c>
       <c r="F480" t="n">
         <v>410.87</v>
@@ -10054,7 +10054,7 @@
         <v>2019.958</v>
       </c>
       <c r="E481" t="n">
-        <v>0.83</v>
+        <v>1.11</v>
       </c>
       <c r="F481" t="n">
         <v>411.76</v>
@@ -10074,7 +10074,7 @@
         <v>2020.042</v>
       </c>
       <c r="E482" t="n">
-        <v>0.83</v>
+        <v>1.16</v>
       </c>
       <c r="F482" t="n">
         <v>412.43</v>
@@ -10094,7 +10094,7 @@
         <v>2020.125</v>
       </c>
       <c r="E483" t="n">
-        <v>0.66</v>
+        <v>1.21</v>
       </c>
       <c r="F483" t="n">
         <v>412.95</v>
@@ -10114,7 +10114,7 @@
         <v>2020.208</v>
       </c>
       <c r="E484" t="n">
-        <v>0.88</v>
+        <v>1.14</v>
       </c>
       <c r="F484" t="n">
         <v>413.44</v>
@@ -10134,7 +10134,7 @@
         <v>2020.292</v>
       </c>
       <c r="E485" t="n">
-        <v>0.8</v>
+        <v>1.13</v>
       </c>
       <c r="F485" t="n">
         <v>413.86</v>
@@ -10154,7 +10154,7 @@
         <v>2020.375</v>
       </c>
       <c r="E486" t="n">
-        <v>0.8100000000000001</v>
+        <v>0.99</v>
       </c>
       <c r="F486" t="n">
         <v>413.81</v>
@@ -10174,7 +10174,7 @@
         <v>2020.458</v>
       </c>
       <c r="E487" t="n">
-        <v>0.84</v>
+        <v>0.93</v>
       </c>
       <c r="F487" t="n">
         <v>412.88</v>
@@ -10194,7 +10194,7 @@
         <v>2020.542</v>
       </c>
       <c r="E488" t="n">
-        <v>0.9</v>
+        <v>0.91</v>
       </c>
       <c r="F488" t="n">
         <v>411.17</v>
@@ -10214,7 +10214,7 @@
         <v>2020.625</v>
       </c>
       <c r="E489" t="n">
-        <v>0.88</v>
+        <v>0.9</v>
       </c>
       <c r="F489" t="n">
         <v>409.73</v>
@@ -10234,7 +10234,7 @@
         <v>2020.708</v>
       </c>
       <c r="E490" t="n">
-        <v>0.93</v>
+        <v>1</v>
       </c>
       <c r="F490" t="n">
         <v>410</v>
@@ -10254,7 +10254,7 @@
         <v>2020.792</v>
       </c>
       <c r="E491" t="n">
-        <v>0.99</v>
+        <v>0.9</v>
       </c>
       <c r="F491" t="n">
         <v>411.66</v>
@@ -10274,7 +10274,7 @@
         <v>2020.875</v>
       </c>
       <c r="E492" t="n">
-        <v>0.93</v>
+        <v>1.06</v>
       </c>
       <c r="F492" t="n">
         <v>413.25</v>
@@ -10294,7 +10294,7 @@
         <v>2020.958</v>
       </c>
       <c r="E493" t="n">
-        <v>0.89</v>
+        <v>0.83</v>
       </c>
       <c r="F493" t="n">
         <v>414.14</v>
@@ -10314,7 +10314,7 @@
         <v>2021.042</v>
       </c>
       <c r="E494" t="n">
-        <v>0.92</v>
+        <v>0.83</v>
       </c>
       <c r="F494" t="n">
         <v>414.74</v>
@@ -10334,7 +10334,7 @@
         <v>2021.125</v>
       </c>
       <c r="E495" t="n">
-        <v>0.9</v>
+        <v>0.66</v>
       </c>
       <c r="F495" t="n">
         <v>415.2</v>
@@ -10354,7 +10354,7 @@
         <v>2021.208</v>
       </c>
       <c r="E496" t="n">
-        <v>1.07</v>
+        <v>0.88</v>
       </c>
       <c r="F496" t="n">
         <v>415.49</v>
@@ -10374,7 +10374,7 @@
         <v>2021.292</v>
       </c>
       <c r="E497" t="n">
-        <v>0.88</v>
+        <v>0.8</v>
       </c>
       <c r="F497" t="n">
         <v>415.81</v>
@@ -10394,7 +10394,7 @@
         <v>2021.375</v>
       </c>
       <c r="E498" t="n">
-        <v>0.82</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="F498" t="n">
         <v>416.01</v>
@@ -10414,7 +10414,7 @@
         <v>2021.458</v>
       </c>
       <c r="E499" t="n">
-        <v>0.92</v>
+        <v>0.84</v>
       </c>
       <c r="F499" t="n">
         <v>415.2</v>
@@ -10454,7 +10454,7 @@
         <v>2021.625</v>
       </c>
       <c r="E501" t="n">
-        <v>0.92</v>
+        <v>0.88</v>
       </c>
       <c r="F501" t="n">
         <v>412.15</v>
@@ -10474,7 +10474,7 @@
         <v>2021.708</v>
       </c>
       <c r="E502" t="n">
-        <v>0.88</v>
+        <v>0.93</v>
       </c>
       <c r="F502" t="n">
         <v>412.38</v>
@@ -10494,7 +10494,7 @@
         <v>2021.792</v>
       </c>
       <c r="E503" t="n">
-        <v>0.96</v>
+        <v>0.99</v>
       </c>
       <c r="F503" t="n">
         <v>413.83</v>
@@ -10514,7 +10514,7 @@
         <v>2021.875</v>
       </c>
       <c r="E504" t="n">
-        <v>0.74</v>
+        <v>0.93</v>
       </c>
       <c r="F504" t="n">
         <v>415.58</v>
@@ -10534,7 +10534,7 @@
         <v>2021.958</v>
       </c>
       <c r="E505" t="n">
-        <v>0.83</v>
+        <v>0.89</v>
       </c>
       <c r="F505" t="n">
         <v>416.61</v>
@@ -10554,7 +10554,7 @@
         <v>2022.042</v>
       </c>
       <c r="E506" t="n">
-        <v>0.89</v>
+        <v>0.92</v>
       </c>
       <c r="F506" t="n">
         <v>417.18</v>
@@ -10574,7 +10574,7 @@
         <v>2022.125</v>
       </c>
       <c r="E507" t="n">
-        <v>1.01</v>
+        <v>0.9</v>
       </c>
       <c r="F507" t="n">
         <v>417.64</v>
@@ -10594,7 +10594,7 @@
         <v>2022.208</v>
       </c>
       <c r="E508" t="n">
-        <v>1.23</v>
+        <v>1.07</v>
       </c>
       <c r="F508" t="n">
         <v>418.16</v>
@@ -10614,7 +10614,7 @@
         <v>2022.292</v>
       </c>
       <c r="E509" t="n">
-        <v>0.99</v>
+        <v>0.88</v>
       </c>
       <c r="F509" t="n">
         <v>418.58</v>
@@ -10634,7 +10634,7 @@
         <v>2022.375</v>
       </c>
       <c r="E510" t="n">
-        <v>0.97</v>
+        <v>0.82</v>
       </c>
       <c r="F510" t="n">
         <v>418.45</v>
@@ -10654,7 +10654,7 @@
         <v>2022.458</v>
       </c>
       <c r="E511" t="n">
-        <v>1.07</v>
+        <v>0.92</v>
       </c>
       <c r="F511" t="n">
         <v>417.43</v>
@@ -10674,7 +10674,7 @@
         <v>2022.542</v>
       </c>
       <c r="E512" t="n">
-        <v>1.18</v>
+        <v>0.9</v>
       </c>
       <c r="F512" t="n">
         <v>415.68</v>
@@ -10694,7 +10694,7 @@
         <v>2022.625</v>
       </c>
       <c r="E513" t="n">
-        <v>1.26</v>
+        <v>0.92</v>
       </c>
       <c r="F513" t="n">
         <v>414.41</v>
@@ -10714,7 +10714,7 @@
         <v>2022.708</v>
       </c>
       <c r="E514" t="n">
-        <v>1.43</v>
+        <v>0.88</v>
       </c>
       <c r="F514" t="n">
         <v>414.63</v>
@@ -10734,7 +10734,7 @@
         <v>2022.792</v>
       </c>
       <c r="E515" t="n">
-        <v>1.37</v>
+        <v>0.96</v>
       </c>
       <c r="F515" t="n">
         <v>416.14</v>
@@ -10754,7 +10754,7 @@
         <v>2022.875</v>
       </c>
       <c r="E516" t="n">
-        <v>1.42</v>
+        <v>0.74</v>
       </c>
       <c r="F516" t="n">
         <v>417.77</v>
@@ -10774,7 +10774,7 @@
         <v>2022.958</v>
       </c>
       <c r="E517" t="n">
-        <v>1.38</v>
+        <v>0.83</v>
       </c>
       <c r="F517" t="n">
         <v>418.8</v>
@@ -10793,7 +10793,9 @@
       <c r="D518" t="n">
         <v>2023.042</v>
       </c>
-      <c r="E518" t="inlineStr"/>
+      <c r="E518" t="n">
+        <v>0.89</v>
+      </c>
       <c r="F518" t="n">
         <v>419.32</v>
       </c>
@@ -10811,7 +10813,9 @@
       <c r="D519" t="n">
         <v>2023.125</v>
       </c>
-      <c r="E519" t="inlineStr"/>
+      <c r="E519" t="n">
+        <v>1.01</v>
+      </c>
       <c r="F519" t="n">
         <v>419.66</v>
       </c>
@@ -10829,7 +10833,9 @@
       <c r="D520" t="n">
         <v>2023.208</v>
       </c>
-      <c r="E520" t="inlineStr"/>
+      <c r="E520" t="n">
+        <v>1.23</v>
+      </c>
       <c r="F520" t="n">
         <v>420.01</v>
       </c>
@@ -10847,7 +10853,9 @@
       <c r="D521" t="n">
         <v>2023.292</v>
       </c>
-      <c r="E521" t="inlineStr"/>
+      <c r="E521" t="n">
+        <v>0.99</v>
+      </c>
       <c r="F521" t="n">
         <v>420.49</v>
       </c>
@@ -10865,7 +10873,9 @@
       <c r="D522" t="n">
         <v>2023.375</v>
       </c>
-      <c r="E522" t="inlineStr"/>
+      <c r="E522" t="n">
+        <v>0.97</v>
+      </c>
       <c r="F522" t="n">
         <v>420.52</v>
       </c>
@@ -10883,7 +10893,9 @@
       <c r="D523" t="n">
         <v>2023.458</v>
       </c>
-      <c r="E523" t="inlineStr"/>
+      <c r="E523" t="n">
+        <v>1.07</v>
+      </c>
       <c r="F523" t="n">
         <v>419.54</v>
       </c>
@@ -10901,7 +10913,9 @@
       <c r="D524" t="n">
         <v>2023.542</v>
       </c>
-      <c r="E524" t="inlineStr"/>
+      <c r="E524" t="n">
+        <v>1.18</v>
+      </c>
       <c r="F524" t="n">
         <v>417.86</v>
       </c>
@@ -10919,7 +10933,9 @@
       <c r="D525" t="n">
         <v>2023.625</v>
       </c>
-      <c r="E525" t="inlineStr"/>
+      <c r="E525" t="n">
+        <v>1.26</v>
+      </c>
       <c r="F525" t="n">
         <v>416.65</v>
       </c>
@@ -10937,7 +10953,9 @@
       <c r="D526" t="n">
         <v>2023.708</v>
       </c>
-      <c r="E526" t="inlineStr"/>
+      <c r="E526" t="n">
+        <v>1.43</v>
+      </c>
       <c r="F526" t="n">
         <v>417.06</v>
       </c>
@@ -10955,7 +10973,9 @@
       <c r="D527" t="n">
         <v>2023.792</v>
       </c>
-      <c r="E527" t="inlineStr"/>
+      <c r="E527" t="n">
+        <v>1.37</v>
+      </c>
       <c r="F527" t="n">
         <v>418.73</v>
       </c>
@@ -10973,7 +10993,9 @@
       <c r="D528" t="n">
         <v>2023.875</v>
       </c>
-      <c r="E528" t="inlineStr"/>
+      <c r="E528" t="n">
+        <v>1.42</v>
+      </c>
       <c r="F528" t="n">
         <v>420.34</v>
       </c>
@@ -10991,7 +11013,9 @@
       <c r="D529" t="n">
         <v>2023.958</v>
       </c>
-      <c r="E529" t="inlineStr"/>
+      <c r="E529" t="n">
+        <v>1.38</v>
+      </c>
       <c r="F529" t="n">
         <v>421.52</v>
       </c>

</xml_diff>